<commit_message>
fix exclusive room for DKV
</commit_message>
<xml_diff>
--- a/out/timetable_result_v3.xlsx
+++ b/out/timetable_result_v3.xlsx
@@ -476,7 +476,7 @@
         <v>BAT, WAH</v>
       </c>
       <c r="F2" t="str">
-        <v>G2-R5</v>
+        <v>B3-R2</v>
       </c>
       <c r="G2" t="str">
         <v>Non-Lab</v>
@@ -488,10 +488,10 @@
         <v>Monday</v>
       </c>
       <c r="J2" t="str">
-        <v>18:30</v>
+        <v>15:30</v>
       </c>
       <c r="K2" t="str">
-        <v>21:00</v>
+        <v>18:00</v>
       </c>
       <c r="L2">
         <v>3</v>
@@ -532,7 +532,7 @@
         <v>ALF, WAH</v>
       </c>
       <c r="F3" t="str">
-        <v>CM-204</v>
+        <v>G3-R1</v>
       </c>
       <c r="G3" t="str">
         <v>Non-Lab</v>
@@ -541,13 +541,13 @@
         <v>No</v>
       </c>
       <c r="I3" t="str">
-        <v>Wednesday</v>
+        <v>Saturday</v>
       </c>
       <c r="J3" t="str">
-        <v>07:30</v>
+        <v>10:50</v>
       </c>
       <c r="K3" t="str">
-        <v>10:00</v>
+        <v>14:10</v>
       </c>
       <c r="L3">
         <v>3</v>
@@ -556,10 +556,10 @@
         <v>150</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O3">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P3">
         <v>15</v>
@@ -588,7 +588,7 @@
         <v>GTK</v>
       </c>
       <c r="F4" t="str">
-        <v>G2-R6</v>
+        <v>CM-208</v>
       </c>
       <c r="G4" t="str">
         <v>Non-Lab</v>
@@ -597,13 +597,13 @@
         <v>No</v>
       </c>
       <c r="I4" t="str">
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="J4" t="str">
-        <v>18:30</v>
+        <v>15:30</v>
       </c>
       <c r="K4" t="str">
-        <v>21:00</v>
+        <v>18:00</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -644,7 +644,7 @@
         <v>BAT</v>
       </c>
       <c r="F5" t="str">
-        <v>G4-R2</v>
+        <v>CM-103</v>
       </c>
       <c r="G5" t="str">
         <v>Non-Lab</v>
@@ -653,13 +653,13 @@
         <v>No</v>
       </c>
       <c r="I5" t="str">
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="J5" t="str">
-        <v>15:30</v>
+        <v>14:10</v>
       </c>
       <c r="K5" t="str">
-        <v>18:00</v>
+        <v>17:10</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -668,10 +668,10 @@
         <v>150</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O5">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="P5">
         <v>15</v>
@@ -700,7 +700,7 @@
         <v>LKT, PTA</v>
       </c>
       <c r="F6" t="str">
-        <v>G2-R6</v>
+        <v>G3-R2</v>
       </c>
       <c r="G6" t="str">
         <v>Non-Lab</v>
@@ -709,7 +709,7 @@
         <v>No</v>
       </c>
       <c r="I6" t="str">
-        <v>Saturday</v>
+        <v>Thursday</v>
       </c>
       <c r="J6" t="str">
         <v>12:30</v>
@@ -756,7 +756,7 @@
         <v>BAT, WAH</v>
       </c>
       <c r="F7" t="str">
-        <v>G2-R4</v>
+        <v>CM-103</v>
       </c>
       <c r="G7" t="str">
         <v>Non-Lab</v>
@@ -768,10 +768,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J7" t="str">
-        <v>10:00</v>
+        <v>12:30</v>
       </c>
       <c r="K7" t="str">
-        <v>13:20</v>
+        <v>15:00</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -780,10 +780,10 @@
         <v>150</v>
       </c>
       <c r="N7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P7">
         <v>15</v>
@@ -812,7 +812,7 @@
         <v>RPA</v>
       </c>
       <c r="F8" t="str">
-        <v>B3-R2</v>
+        <v>G3-R1</v>
       </c>
       <c r="G8" t="str">
         <v>Non-Lab</v>
@@ -821,13 +821,13 @@
         <v>No</v>
       </c>
       <c r="I8" t="str">
-        <v>Wednesday</v>
+        <v>Saturday</v>
       </c>
       <c r="J8" t="str">
-        <v>10:00</v>
+        <v>08:20</v>
       </c>
       <c r="K8" t="str">
-        <v>13:20</v>
+        <v>10:50</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -836,10 +836,10 @@
         <v>150</v>
       </c>
       <c r="N8">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P8">
         <v>15</v>
@@ -868,7 +868,7 @@
         <v>RPA, ELD</v>
       </c>
       <c r="F9" t="str">
-        <v>CM-101</v>
+        <v>G2-R2</v>
       </c>
       <c r="G9" t="str">
         <v>Non-Lab</v>
@@ -877,7 +877,7 @@
         <v>No</v>
       </c>
       <c r="I9" t="str">
-        <v>Saturday</v>
+        <v>Monday</v>
       </c>
       <c r="J9" t="str">
         <v>18:30</v>
@@ -924,7 +924,7 @@
         <v>GFP</v>
       </c>
       <c r="F10" t="str">
-        <v>G4-R3</v>
+        <v>B3-R2</v>
       </c>
       <c r="G10" t="str">
         <v>Non-Lab</v>
@@ -933,13 +933,13 @@
         <v>No</v>
       </c>
       <c r="I10" t="str">
-        <v>Thursday</v>
+        <v>Friday</v>
       </c>
       <c r="J10" t="str">
-        <v>16:20</v>
+        <v>18:30</v>
       </c>
       <c r="K10" t="str">
-        <v>19:20</v>
+        <v>21:00</v>
       </c>
       <c r="L10">
         <v>3</v>
@@ -948,10 +948,10 @@
         <v>150</v>
       </c>
       <c r="N10">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P10">
         <v>15</v>
@@ -980,7 +980,7 @@
         <v>ALF, WKS</v>
       </c>
       <c r="F11" t="str">
-        <v>G2-R6</v>
+        <v>G3-R4</v>
       </c>
       <c r="G11" t="str">
         <v>Non-Lab</v>
@@ -989,13 +989,13 @@
         <v>No</v>
       </c>
       <c r="I11" t="str">
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="J11" t="str">
-        <v>15:30</v>
+        <v>08:20</v>
       </c>
       <c r="K11" t="str">
-        <v>18:00</v>
+        <v>10:50</v>
       </c>
       <c r="L11">
         <v>3</v>
@@ -1036,7 +1036,7 @@
         <v>GTK</v>
       </c>
       <c r="F12" t="str">
-        <v>G3-R4</v>
+        <v>CM-201</v>
       </c>
       <c r="G12" t="str">
         <v>Non-Lab</v>
@@ -1045,13 +1045,13 @@
         <v>No</v>
       </c>
       <c r="I12" t="str">
-        <v>Wednesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J12" t="str">
-        <v>15:30</v>
+        <v>18:30</v>
       </c>
       <c r="K12" t="str">
-        <v>18:00</v>
+        <v>21:00</v>
       </c>
       <c r="L12">
         <v>3</v>
@@ -1104,10 +1104,10 @@
         <v>Saturday</v>
       </c>
       <c r="J13" t="str">
-        <v>09:10</v>
+        <v>15:30</v>
       </c>
       <c r="K13" t="str">
-        <v>11:40</v>
+        <v>18:00</v>
       </c>
       <c r="L13">
         <v>3</v>
@@ -1148,7 +1148,7 @@
         <v>WKS, ELD</v>
       </c>
       <c r="F14" t="str">
-        <v>G2-R7</v>
+        <v>G2-R2</v>
       </c>
       <c r="G14" t="str">
         <v>Non-Lab</v>
@@ -1157,13 +1157,13 @@
         <v>No</v>
       </c>
       <c r="I14" t="str">
-        <v>Tuesday</v>
+        <v>Monday</v>
       </c>
       <c r="J14" t="str">
-        <v>13:20</v>
+        <v>07:30</v>
       </c>
       <c r="K14" t="str">
-        <v>16:20</v>
+        <v>10:00</v>
       </c>
       <c r="L14">
         <v>3</v>
@@ -1172,10 +1172,10 @@
         <v>150</v>
       </c>
       <c r="N14">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P14">
         <v>30</v>
@@ -1204,7 +1204,7 @@
         <v>PTA, WND</v>
       </c>
       <c r="F15" t="str">
-        <v>B3-R1</v>
+        <v>G2-R4</v>
       </c>
       <c r="G15" t="str">
         <v>Non-Lab</v>
@@ -1213,13 +1213,13 @@
         <v>No</v>
       </c>
       <c r="I15" t="str">
-        <v>Thursday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J15" t="str">
-        <v>12:30</v>
+        <v>07:30</v>
       </c>
       <c r="K15" t="str">
-        <v>15:00</v>
+        <v>10:00</v>
       </c>
       <c r="L15">
         <v>3</v>
@@ -1260,7 +1260,7 @@
         <v>MAL</v>
       </c>
       <c r="F16" t="str">
-        <v>CM-208</v>
+        <v>CM-202</v>
       </c>
       <c r="G16" t="str">
         <v>Non-Lab</v>
@@ -1316,7 +1316,7 @@
         <v>AWD</v>
       </c>
       <c r="F17" t="str">
-        <v>CM-202</v>
+        <v>CM-203</v>
       </c>
       <c r="G17" t="str">
         <v>Non-Lab</v>
@@ -1325,13 +1325,13 @@
         <v>No</v>
       </c>
       <c r="I17" t="str">
-        <v>Thursday</v>
+        <v>Monday</v>
       </c>
       <c r="J17" t="str">
-        <v>07:30</v>
+        <v>10:00</v>
       </c>
       <c r="K17" t="str">
-        <v>10:00</v>
+        <v>13:20</v>
       </c>
       <c r="L17">
         <v>3</v>
@@ -1340,10 +1340,10 @@
         <v>150</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O17">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P17">
         <v>45</v>
@@ -1372,7 +1372,7 @@
         <v>ALF</v>
       </c>
       <c r="F18" t="str">
-        <v>G4-R3</v>
+        <v>CM-208</v>
       </c>
       <c r="G18" t="str">
         <v>Non-Lab</v>
@@ -1428,7 +1428,7 @@
         <v>ALF</v>
       </c>
       <c r="F19" t="str">
-        <v>CM-203</v>
+        <v>G4-R2</v>
       </c>
       <c r="G19" t="str">
         <v>Non-Lab</v>
@@ -1493,7 +1493,7 @@
         <v>No</v>
       </c>
       <c r="I20" t="str">
-        <v>Tuesday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J20" t="str">
         <v>07:30</v>
@@ -1540,7 +1540,7 @@
         <v>HDC</v>
       </c>
       <c r="F21" t="str">
-        <v>CM-203</v>
+        <v>CM-208</v>
       </c>
       <c r="G21" t="str">
         <v>Non-Lab</v>
@@ -1596,7 +1596,7 @@
         <v>HDC</v>
       </c>
       <c r="F22" t="str">
-        <v>G4-R4</v>
+        <v>G4-R1</v>
       </c>
       <c r="G22" t="str">
         <v>Non-Lab</v>
@@ -1652,7 +1652,7 @@
         <v>HDC</v>
       </c>
       <c r="F23" t="str">
-        <v>CM-202</v>
+        <v>G4-R3</v>
       </c>
       <c r="G23" t="str">
         <v>Non-Lab</v>
@@ -1661,13 +1661,13 @@
         <v>No</v>
       </c>
       <c r="I23" t="str">
-        <v>Monday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J23" t="str">
-        <v>10:00</v>
+        <v>16:20</v>
       </c>
       <c r="K23" t="str">
-        <v>11:40</v>
+        <v>18:00</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -1717,7 +1717,7 @@
         <v>No</v>
       </c>
       <c r="I24" t="str">
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J24" t="str">
         <v>07:30</v>
@@ -1764,7 +1764,7 @@
         <v>ADL</v>
       </c>
       <c r="F25" t="str">
-        <v>G4-R1</v>
+        <v>G4-R3</v>
       </c>
       <c r="G25" t="str">
         <v>Non-Lab</v>
@@ -1820,7 +1820,7 @@
         <v>LRS</v>
       </c>
       <c r="F26" t="str">
-        <v>CM-101</v>
+        <v>CM-102</v>
       </c>
       <c r="G26" t="str">
         <v>Non-Lab</v>
@@ -1876,7 +1876,7 @@
         <v>ZSR</v>
       </c>
       <c r="F27" t="str">
-        <v>CM-202</v>
+        <v>CM-203</v>
       </c>
       <c r="G27" t="str">
         <v>Non-Lab</v>
@@ -1941,13 +1941,13 @@
         <v>No</v>
       </c>
       <c r="I28" t="str">
-        <v>Tuesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J28" t="str">
-        <v>15:30</v>
+        <v>07:30</v>
       </c>
       <c r="K28" t="str">
-        <v>18:00</v>
+        <v>10:00</v>
       </c>
       <c r="L28">
         <v>3</v>
@@ -1988,7 +1988,7 @@
         <v>ANW</v>
       </c>
       <c r="F29" t="str">
-        <v>CM-202</v>
+        <v>CM-103</v>
       </c>
       <c r="G29" t="str">
         <v>Non-Lab</v>
@@ -2044,7 +2044,7 @@
         <v>AWP</v>
       </c>
       <c r="F30" t="str">
-        <v>CM-208</v>
+        <v>G4-R4</v>
       </c>
       <c r="G30" t="str">
         <v>Non-Lab</v>
@@ -2156,7 +2156,7 @@
         <v>MDI</v>
       </c>
       <c r="F32" t="str">
-        <v>CM-101</v>
+        <v>CM-205</v>
       </c>
       <c r="G32" t="str">
         <v>Non-Lab</v>
@@ -2212,7 +2212,7 @@
         <v>MDI</v>
       </c>
       <c r="F33" t="str">
-        <v>CM-208</v>
+        <v>CM-102</v>
       </c>
       <c r="G33" t="str">
         <v>Non-Lab</v>
@@ -2224,10 +2224,10 @@
         <v>Friday</v>
       </c>
       <c r="J33" t="str">
-        <v>08:20</v>
+        <v>07:30</v>
       </c>
       <c r="K33" t="str">
-        <v>10:50</v>
+        <v>10:00</v>
       </c>
       <c r="L33">
         <v>3</v>
@@ -2268,7 +2268,7 @@
         <v>ANW</v>
       </c>
       <c r="F34" t="str">
-        <v>CM-202</v>
+        <v>CM-203</v>
       </c>
       <c r="G34" t="str">
         <v>Non-Lab</v>
@@ -2324,7 +2324,7 @@
         <v>MMK</v>
       </c>
       <c r="F35" t="str">
-        <v>G3-R1</v>
+        <v>CM-205</v>
       </c>
       <c r="G35" t="str">
         <v>Non-Lab</v>
@@ -2380,7 +2380,7 @@
         <v>MMK</v>
       </c>
       <c r="F36" t="str">
-        <v>CM-101</v>
+        <v>CM-203</v>
       </c>
       <c r="G36" t="str">
         <v>Non-Lab</v>
@@ -2436,7 +2436,7 @@
         <v>FRD</v>
       </c>
       <c r="F37" t="str">
-        <v>CM-101</v>
+        <v>CM-203</v>
       </c>
       <c r="G37" t="str">
         <v>Non-Lab</v>
@@ -2492,7 +2492,7 @@
         <v>AWD</v>
       </c>
       <c r="F38" t="str">
-        <v>CM-201</v>
+        <v>CM-202</v>
       </c>
       <c r="G38" t="str">
         <v>Non-Lab</v>
@@ -2548,7 +2548,7 @@
         <v>FRD</v>
       </c>
       <c r="F39" t="str">
-        <v>CM-208</v>
+        <v>CM-205</v>
       </c>
       <c r="G39" t="str">
         <v>Non-Lab</v>
@@ -2557,13 +2557,13 @@
         <v>No</v>
       </c>
       <c r="I39" t="str">
-        <v>Monday</v>
+        <v>Thursday</v>
       </c>
       <c r="J39" t="str">
-        <v>10:00</v>
+        <v>16:20</v>
       </c>
       <c r="K39" t="str">
-        <v>13:20</v>
+        <v>19:20</v>
       </c>
       <c r="L39">
         <v>3</v>
@@ -2572,10 +2572,10 @@
         <v>150</v>
       </c>
       <c r="N39">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="O39">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="P39">
         <v>45</v>
@@ -2604,7 +2604,7 @@
         <v>IKN</v>
       </c>
       <c r="F40" t="str">
-        <v>CM-208</v>
+        <v>CM-102</v>
       </c>
       <c r="G40" t="str">
         <v>Non-Lab</v>
@@ -2660,7 +2660,7 @@
         <v>LRS</v>
       </c>
       <c r="F41" t="str">
-        <v>CM-201</v>
+        <v>CM-103</v>
       </c>
       <c r="G41" t="str">
         <v>Non-Lab</v>
@@ -2772,7 +2772,7 @@
         <v>ADL</v>
       </c>
       <c r="F43" t="str">
-        <v>CM-201</v>
+        <v>CM-204</v>
       </c>
       <c r="G43" t="str">
         <v>Non-Lab</v>
@@ -2828,7 +2828,7 @@
         <v>ADL</v>
       </c>
       <c r="F44" t="str">
-        <v>G4-R4</v>
+        <v>CM-208</v>
       </c>
       <c r="G44" t="str">
         <v>Non-Lab</v>
@@ -2837,13 +2837,13 @@
         <v>No</v>
       </c>
       <c r="I44" t="str">
-        <v>Tuesday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J44" t="str">
+        <v>13:20</v>
+      </c>
+      <c r="K44" t="str">
         <v>16:20</v>
-      </c>
-      <c r="K44" t="str">
-        <v>19:20</v>
       </c>
       <c r="L44">
         <v>3</v>
@@ -2893,13 +2893,13 @@
         <v>No</v>
       </c>
       <c r="I45" t="str">
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J45" t="str">
-        <v>07:30</v>
+        <v>16:20</v>
       </c>
       <c r="K45" t="str">
-        <v>10:00</v>
+        <v>19:20</v>
       </c>
       <c r="L45">
         <v>3</v>
@@ -2908,10 +2908,10 @@
         <v>150</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O45">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="P45">
         <v>40</v>
@@ -2940,7 +2940,7 @@
         <v>MAK</v>
       </c>
       <c r="F46" t="str">
-        <v>CM-101</v>
+        <v>G4-R1</v>
       </c>
       <c r="G46" t="str">
         <v>Non-Lab</v>
@@ -2996,7 +2996,7 @@
         <v>FRD</v>
       </c>
       <c r="F47" t="str">
-        <v>CM-201</v>
+        <v>CM-202</v>
       </c>
       <c r="G47" t="str">
         <v>Non-Lab</v>
@@ -3008,10 +3008,10 @@
         <v>Wednesday</v>
       </c>
       <c r="J47" t="str">
-        <v>13:20</v>
+        <v>07:30</v>
       </c>
       <c r="K47" t="str">
-        <v>16:20</v>
+        <v>10:00</v>
       </c>
       <c r="L47">
         <v>3</v>
@@ -3020,10 +3020,10 @@
         <v>150</v>
       </c>
       <c r="N47">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O47">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P47">
         <v>40</v>
@@ -3052,7 +3052,7 @@
         <v>AWD</v>
       </c>
       <c r="F48" t="str">
-        <v>G4-R3</v>
+        <v>G4-R2</v>
       </c>
       <c r="G48" t="str">
         <v>Non-Lab</v>
@@ -3108,7 +3108,7 @@
         <v>ADL</v>
       </c>
       <c r="F49" t="str">
-        <v>CM-203</v>
+        <v>CM-201</v>
       </c>
       <c r="G49" t="str">
         <v>Non-Lab</v>
@@ -3220,7 +3220,7 @@
         <v>AFT</v>
       </c>
       <c r="F51" t="str">
-        <v>CM-201</v>
+        <v>CM-208</v>
       </c>
       <c r="G51" t="str">
         <v>Non-Lab</v>
@@ -3276,7 +3276,7 @@
         <v>FRD</v>
       </c>
       <c r="F52" t="str">
-        <v>CM-203</v>
+        <v>CM-204</v>
       </c>
       <c r="G52" t="str">
         <v>Non-Lab</v>
@@ -3285,13 +3285,13 @@
         <v>No</v>
       </c>
       <c r="I52" t="str">
-        <v>Thursday</v>
+        <v>Monday</v>
       </c>
       <c r="J52" t="str">
-        <v>16:20</v>
+        <v>10:00</v>
       </c>
       <c r="K52" t="str">
-        <v>19:20</v>
+        <v>13:20</v>
       </c>
       <c r="L52">
         <v>3</v>
@@ -3300,10 +3300,10 @@
         <v>150</v>
       </c>
       <c r="N52">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O52">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="P52">
         <v>42</v>
@@ -3332,7 +3332,7 @@
         <v>AFT</v>
       </c>
       <c r="F53" t="str">
-        <v>CM-102</v>
+        <v>CM-204</v>
       </c>
       <c r="G53" t="str">
         <v>Non-Lab</v>
@@ -3344,10 +3344,10 @@
         <v>Friday</v>
       </c>
       <c r="J53" t="str">
-        <v>07:30</v>
+        <v>14:10</v>
       </c>
       <c r="K53" t="str">
-        <v>10:00</v>
+        <v>17:10</v>
       </c>
       <c r="L53">
         <v>3</v>
@@ -3356,10 +3356,10 @@
         <v>150</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O53">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="P53">
         <v>42</v>
@@ -3400,10 +3400,10 @@
         <v>Friday</v>
       </c>
       <c r="J54" t="str">
-        <v>10:00</v>
+        <v>10:50</v>
       </c>
       <c r="K54" t="str">
-        <v>13:20</v>
+        <v>14:10</v>
       </c>
       <c r="L54">
         <v>3</v>
@@ -3444,7 +3444,7 @@
         <v>MAK</v>
       </c>
       <c r="F55" t="str">
-        <v>G4-R2</v>
+        <v>G4-R4</v>
       </c>
       <c r="G55" t="str">
         <v>Non-Lab</v>
@@ -3456,10 +3456,10 @@
         <v>Friday</v>
       </c>
       <c r="J55" t="str">
-        <v>15:30</v>
+        <v>07:30</v>
       </c>
       <c r="K55" t="str">
-        <v>18:00</v>
+        <v>10:00</v>
       </c>
       <c r="L55">
         <v>3</v>
@@ -3500,7 +3500,7 @@
         <v>MAL</v>
       </c>
       <c r="F56" t="str">
-        <v>G3-R1</v>
+        <v>B3-R2</v>
       </c>
       <c r="G56" t="str">
         <v>Non-Lab</v>
@@ -3509,13 +3509,13 @@
         <v>No</v>
       </c>
       <c r="I56" t="str">
-        <v>Monday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J56" t="str">
-        <v>10:00</v>
+        <v>12:30</v>
       </c>
       <c r="K56" t="str">
-        <v>13:20</v>
+        <v>15:00</v>
       </c>
       <c r="L56">
         <v>3</v>
@@ -3524,10 +3524,10 @@
         <v>150</v>
       </c>
       <c r="N56">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O56">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P56">
         <v>25</v>
@@ -3556,7 +3556,7 @@
         <v>MAL</v>
       </c>
       <c r="F57" t="str">
-        <v>G3-R4</v>
+        <v>G2-R7</v>
       </c>
       <c r="G57" t="str">
         <v>Non-Lab</v>
@@ -3565,13 +3565,13 @@
         <v>No</v>
       </c>
       <c r="I57" t="str">
-        <v>Wednesday</v>
+        <v>Monday</v>
       </c>
       <c r="J57" t="str">
-        <v>07:30</v>
+        <v>13:20</v>
       </c>
       <c r="K57" t="str">
-        <v>10:00</v>
+        <v>16:20</v>
       </c>
       <c r="L57">
         <v>3</v>
@@ -3580,10 +3580,10 @@
         <v>150</v>
       </c>
       <c r="N57">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O57">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="P57">
         <v>25</v>
@@ -3612,7 +3612,7 @@
         <v>EMH</v>
       </c>
       <c r="F58" t="str">
-        <v>G3-R4</v>
+        <v>G2-R2</v>
       </c>
       <c r="G58" t="str">
         <v>Non-Lab</v>
@@ -3621,7 +3621,7 @@
         <v>No</v>
       </c>
       <c r="I58" t="str">
-        <v>Monday</v>
+        <v>Friday</v>
       </c>
       <c r="J58" t="str">
         <v>07:30</v>
@@ -3668,7 +3668,7 @@
         <v>ADM</v>
       </c>
       <c r="F59" t="str">
-        <v>B2-R1</v>
+        <v>G2-R2</v>
       </c>
       <c r="G59" t="str">
         <v>Non-Lab</v>
@@ -3677,13 +3677,13 @@
         <v>No</v>
       </c>
       <c r="I59" t="str">
-        <v>Monday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J59" t="str">
-        <v>16:20</v>
+        <v>07:30</v>
       </c>
       <c r="K59" t="str">
-        <v>19:20</v>
+        <v>10:00</v>
       </c>
       <c r="L59">
         <v>3</v>
@@ -3692,10 +3692,10 @@
         <v>150</v>
       </c>
       <c r="N59">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O59">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P59">
         <v>25</v>
@@ -3724,7 +3724,7 @@
         <v>MHA</v>
       </c>
       <c r="F60" t="str">
-        <v>CM-202</v>
+        <v>CM-203</v>
       </c>
       <c r="G60" t="str">
         <v>Non-Lab</v>
@@ -3733,13 +3733,13 @@
         <v>No</v>
       </c>
       <c r="I60" t="str">
-        <v>Tuesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J60" t="str">
-        <v>07:30</v>
+        <v>14:10</v>
       </c>
       <c r="K60" t="str">
-        <v>09:10</v>
+        <v>16:20</v>
       </c>
       <c r="L60">
         <v>2</v>
@@ -3748,10 +3748,10 @@
         <v>100</v>
       </c>
       <c r="N60">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O60">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P60">
         <v>25</v>
@@ -3780,7 +3780,7 @@
         <v>ADM</v>
       </c>
       <c r="F61" t="str">
-        <v>CM-101</v>
+        <v>CM-203</v>
       </c>
       <c r="G61" t="str">
         <v>Non-Lab</v>
@@ -3836,7 +3836,7 @@
         <v>EMH</v>
       </c>
       <c r="F62" t="str">
-        <v>G3-R4</v>
+        <v>G2-R4</v>
       </c>
       <c r="G62" t="str">
         <v>Non-Lab</v>
@@ -3845,13 +3845,13 @@
         <v>No</v>
       </c>
       <c r="I62" t="str">
-        <v>Tuesday</v>
+        <v>Monday</v>
       </c>
       <c r="J62" t="str">
-        <v>12:30</v>
+        <v>10:00</v>
       </c>
       <c r="K62" t="str">
-        <v>15:00</v>
+        <v>13:20</v>
       </c>
       <c r="L62">
         <v>3</v>
@@ -3860,10 +3860,10 @@
         <v>150</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O62">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P62">
         <v>30</v>
@@ -3892,7 +3892,7 @@
         <v>MHA</v>
       </c>
       <c r="F63" t="str">
-        <v>B2-R1</v>
+        <v>CM-102</v>
       </c>
       <c r="G63" t="str">
         <v>Non-Lab</v>
@@ -3948,7 +3948,7 @@
         <v>ADM</v>
       </c>
       <c r="F64" t="str">
-        <v>G2-R3</v>
+        <v>CM-203</v>
       </c>
       <c r="G64" t="str">
         <v>Non-Lab</v>
@@ -3960,10 +3960,10 @@
         <v>Monday</v>
       </c>
       <c r="J64" t="str">
-        <v>13:20</v>
+        <v>16:20</v>
       </c>
       <c r="K64" t="str">
-        <v>16:20</v>
+        <v>19:20</v>
       </c>
       <c r="L64">
         <v>3</v>
@@ -4004,7 +4004,7 @@
         <v>WAH</v>
       </c>
       <c r="F65" t="str">
-        <v>CM-201</v>
+        <v>G2-R6</v>
       </c>
       <c r="G65" t="str">
         <v>Non-Lab</v>
@@ -4060,7 +4060,7 @@
         <v>MHA</v>
       </c>
       <c r="F66" t="str">
-        <v>CM-204</v>
+        <v>G3-R4</v>
       </c>
       <c r="G66" t="str">
         <v>Non-Lab</v>
@@ -4069,13 +4069,13 @@
         <v>No</v>
       </c>
       <c r="I66" t="str">
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J66" t="str">
-        <v>07:30</v>
+        <v>13:20</v>
       </c>
       <c r="K66" t="str">
-        <v>10:00</v>
+        <v>16:20</v>
       </c>
       <c r="L66">
         <v>3</v>
@@ -4084,10 +4084,10 @@
         <v>150</v>
       </c>
       <c r="N66">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O66">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="P66">
         <v>30</v>
@@ -4116,7 +4116,7 @@
         <v>WAH</v>
       </c>
       <c r="F67" t="str">
-        <v>G2-R6</v>
+        <v>G4-R3</v>
       </c>
       <c r="G67" t="str">
         <v>Non-Lab</v>
@@ -4125,13 +4125,13 @@
         <v>No</v>
       </c>
       <c r="I67" t="str">
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J67" t="str">
-        <v>13:20</v>
+        <v>07:30</v>
       </c>
       <c r="K67" t="str">
-        <v>15:00</v>
+        <v>09:10</v>
       </c>
       <c r="L67">
         <v>2</v>
@@ -4172,7 +4172,7 @@
         <v>EMH</v>
       </c>
       <c r="F68" t="str">
-        <v>CM-208</v>
+        <v>CM-202</v>
       </c>
       <c r="G68" t="str">
         <v>Non-Lab</v>
@@ -4181,13 +4181,13 @@
         <v>No</v>
       </c>
       <c r="I68" t="str">
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J68" t="str">
-        <v>07:30</v>
+        <v>16:20</v>
       </c>
       <c r="K68" t="str">
-        <v>09:10</v>
+        <v>18:00</v>
       </c>
       <c r="L68">
         <v>2</v>
@@ -4228,7 +4228,7 @@
         <v>BAT</v>
       </c>
       <c r="F69" t="str">
-        <v>G2-R2</v>
+        <v>G2-R5</v>
       </c>
       <c r="G69" t="str">
         <v>Non-Lab</v>
@@ -4284,7 +4284,7 @@
         <v>WAH</v>
       </c>
       <c r="F70" t="str">
-        <v>G3-R4</v>
+        <v>G2-R5</v>
       </c>
       <c r="G70" t="str">
         <v>Non-Lab</v>
@@ -4296,10 +4296,10 @@
         <v>Thursday</v>
       </c>
       <c r="J70" t="str">
-        <v>12:30</v>
+        <v>07:30</v>
       </c>
       <c r="K70" t="str">
-        <v>14:10</v>
+        <v>09:10</v>
       </c>
       <c r="L70">
         <v>2</v>
@@ -4340,7 +4340,7 @@
         <v>MHA</v>
       </c>
       <c r="F71" t="str">
-        <v>CM-101</v>
+        <v>G2-R7</v>
       </c>
       <c r="G71" t="str">
         <v>Non-Lab</v>
@@ -4352,10 +4352,10 @@
         <v>Thursday</v>
       </c>
       <c r="J71" t="str">
+        <v>12:30</v>
+      </c>
+      <c r="K71" t="str">
         <v>14:10</v>
-      </c>
-      <c r="K71" t="str">
-        <v>16:20</v>
       </c>
       <c r="L71">
         <v>2</v>
@@ -4364,10 +4364,10 @@
         <v>100</v>
       </c>
       <c r="N71">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O71">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="P71">
         <v>25</v>
@@ -4396,7 +4396,7 @@
         <v>BAT</v>
       </c>
       <c r="F72" t="str">
-        <v>G3-R2</v>
+        <v>G2-R6</v>
       </c>
       <c r="G72" t="str">
         <v>Non-Lab</v>
@@ -4452,7 +4452,7 @@
         <v>ADM</v>
       </c>
       <c r="F73" t="str">
-        <v>CM-201</v>
+        <v>CM-102</v>
       </c>
       <c r="G73" t="str">
         <v>Non-Lab</v>
@@ -4461,13 +4461,13 @@
         <v>No</v>
       </c>
       <c r="I73" t="str">
-        <v>Wednesday</v>
+        <v>Monday</v>
       </c>
       <c r="J73" t="str">
-        <v>16:20</v>
+        <v>07:30</v>
       </c>
       <c r="K73" t="str">
-        <v>19:20</v>
+        <v>10:00</v>
       </c>
       <c r="L73">
         <v>3</v>
@@ -4476,10 +4476,10 @@
         <v>150</v>
       </c>
       <c r="N73">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O73">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P73">
         <v>25</v>
@@ -4508,7 +4508,7 @@
         <v>JSM</v>
       </c>
       <c r="F74" t="str">
-        <v>G4-R1</v>
+        <v>CM-204</v>
       </c>
       <c r="G74" t="str">
         <v>Non-Lab</v>
@@ -4564,7 +4564,7 @@
         <v>ADM</v>
       </c>
       <c r="F75" t="str">
-        <v>CM-205</v>
+        <v>G3-R4</v>
       </c>
       <c r="G75" t="str">
         <v>Non-Lab</v>
@@ -4620,7 +4620,7 @@
         <v>AAV</v>
       </c>
       <c r="F76" t="str">
-        <v>CM-205</v>
+        <v>CM-201</v>
       </c>
       <c r="G76" t="str">
         <v>Non-Lab</v>
@@ -4629,7 +4629,7 @@
         <v>No</v>
       </c>
       <c r="I76" t="str">
-        <v>Tuesday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J76" t="str">
         <v>15:30</v>
@@ -4676,7 +4676,7 @@
         <v>NCS</v>
       </c>
       <c r="F77" t="str">
-        <v>CM-103</v>
+        <v>CM-101</v>
       </c>
       <c r="G77" t="str">
         <v>Non-Lab</v>
@@ -4685,13 +4685,13 @@
         <v>No</v>
       </c>
       <c r="I77" t="str">
-        <v>Thursday</v>
+        <v>Monday</v>
       </c>
       <c r="J77" t="str">
-        <v>07:30</v>
+        <v>10:00</v>
       </c>
       <c r="K77" t="str">
-        <v>10:00</v>
+        <v>13:20</v>
       </c>
       <c r="L77">
         <v>3</v>
@@ -4700,10 +4700,10 @@
         <v>150</v>
       </c>
       <c r="N77">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O77">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P77">
         <v>40</v>
@@ -4732,7 +4732,7 @@
         <v>NCS</v>
       </c>
       <c r="F78" t="str">
-        <v>CM-103</v>
+        <v>CM-208</v>
       </c>
       <c r="G78" t="str">
         <v>Non-Lab</v>
@@ -4741,13 +4741,13 @@
         <v>No</v>
       </c>
       <c r="I78" t="str">
-        <v>Monday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J78" t="str">
-        <v>12:30</v>
+        <v>10:00</v>
       </c>
       <c r="K78" t="str">
-        <v>15:00</v>
+        <v>13:20</v>
       </c>
       <c r="L78">
         <v>3</v>
@@ -4756,10 +4756,10 @@
         <v>150</v>
       </c>
       <c r="N78">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O78">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P78">
         <v>40</v>
@@ -4788,7 +4788,7 @@
         <v>NWF</v>
       </c>
       <c r="F79" t="str">
-        <v>CM-206</v>
+        <v>CM-LabVirtual</v>
       </c>
       <c r="G79" t="str">
         <v>Lab</v>
@@ -4797,13 +4797,13 @@
         <v>No</v>
       </c>
       <c r="I79" t="str">
-        <v>Thursday</v>
+        <v>Monday</v>
       </c>
       <c r="J79" t="str">
-        <v>12:30</v>
+        <v>15:30</v>
       </c>
       <c r="K79" t="str">
-        <v>15:00</v>
+        <v>18:00</v>
       </c>
       <c r="L79">
         <v>3</v>
@@ -4844,7 +4844,7 @@
         <v>AHY</v>
       </c>
       <c r="F80" t="str">
-        <v>CM-205</v>
+        <v>CM-202</v>
       </c>
       <c r="G80" t="str">
         <v>Non-Lab</v>
@@ -4853,7 +4853,7 @@
         <v>No</v>
       </c>
       <c r="I80" t="str">
-        <v>Tuesday</v>
+        <v>Friday</v>
       </c>
       <c r="J80" t="str">
         <v>07:30</v>
@@ -4900,7 +4900,7 @@
         <v>MAF</v>
       </c>
       <c r="F81" t="str">
-        <v>CM-205</v>
+        <v>G4-R1</v>
       </c>
       <c r="G81" t="str">
         <v>Non-Lab</v>
@@ -4909,14 +4909,14 @@
         <v>No</v>
       </c>
       <c r="I81" t="str">
-        <v>Tuesday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J81" t="str">
+        <v>07:30</v>
+      </c>
+      <c r="K81" t="str">
         <v>10:00</v>
       </c>
-      <c r="K81" t="str">
-        <v>13:20</v>
-      </c>
       <c r="L81">
         <v>3</v>
       </c>
@@ -4924,10 +4924,10 @@
         <v>150</v>
       </c>
       <c r="N81">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O81">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P81">
         <v>40</v>
@@ -4956,7 +4956,7 @@
         <v>AAV</v>
       </c>
       <c r="F82" t="str">
-        <v>B2-R1</v>
+        <v>G2-R3</v>
       </c>
       <c r="G82" t="str">
         <v>Non-Lab</v>
@@ -4968,10 +4968,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J82" t="str">
-        <v>18:30</v>
+        <v>15:30</v>
       </c>
       <c r="K82" t="str">
-        <v>21:00</v>
+        <v>18:00</v>
       </c>
       <c r="L82">
         <v>3</v>
@@ -5012,7 +5012,7 @@
         <v>NCS</v>
       </c>
       <c r="F83" t="str">
-        <v>G2-R3</v>
+        <v>G2-R5</v>
       </c>
       <c r="G83" t="str">
         <v>Non-Lab</v>
@@ -5021,7 +5021,7 @@
         <v>No</v>
       </c>
       <c r="I83" t="str">
-        <v>Wednesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J83" t="str">
         <v>18:30</v>
@@ -5068,7 +5068,7 @@
         <v>NCS</v>
       </c>
       <c r="F84" t="str">
-        <v>G3-R1</v>
+        <v>G3-R2</v>
       </c>
       <c r="G84" t="str">
         <v>Non-Lab</v>
@@ -5124,7 +5124,7 @@
         <v>NWF</v>
       </c>
       <c r="F85" t="str">
-        <v>CM-202</v>
+        <v>CM-204</v>
       </c>
       <c r="G85" t="str">
         <v>Non-Lab</v>
@@ -5133,7 +5133,7 @@
         <v>No</v>
       </c>
       <c r="I85" t="str">
-        <v>Thursday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J85" t="str">
         <v>18:30</v>
@@ -5180,7 +5180,7 @@
         <v>AHY</v>
       </c>
       <c r="F86" t="str">
-        <v>CM-103</v>
+        <v>G3-R2</v>
       </c>
       <c r="G86" t="str">
         <v>Non-Lab</v>
@@ -5189,7 +5189,7 @@
         <v>No</v>
       </c>
       <c r="I86" t="str">
-        <v>Friday</v>
+        <v>Monday</v>
       </c>
       <c r="J86" t="str">
         <v>18:30</v>
@@ -5236,7 +5236,7 @@
         <v>MAF</v>
       </c>
       <c r="F87" t="str">
-        <v>B2-R1</v>
+        <v>CM-201</v>
       </c>
       <c r="G87" t="str">
         <v>Non-Lab</v>
@@ -5245,13 +5245,13 @@
         <v>No</v>
       </c>
       <c r="I87" t="str">
-        <v>Wednesday</v>
+        <v>Friday</v>
       </c>
       <c r="J87" t="str">
-        <v>15:30</v>
+        <v>18:30</v>
       </c>
       <c r="K87" t="str">
-        <v>18:00</v>
+        <v>21:00</v>
       </c>
       <c r="L87">
         <v>3</v>
@@ -5292,7 +5292,7 @@
         <v>AAV</v>
       </c>
       <c r="F88" t="str">
-        <v>CM-101</v>
+        <v>G3-R4</v>
       </c>
       <c r="G88" t="str">
         <v>Non-Lab</v>
@@ -5348,7 +5348,7 @@
         <v>NCS</v>
       </c>
       <c r="F89" t="str">
-        <v>G3-R2</v>
+        <v>G3-R4</v>
       </c>
       <c r="G89" t="str">
         <v>Non-Lab</v>
@@ -5357,13 +5357,13 @@
         <v>No</v>
       </c>
       <c r="I89" t="str">
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J89" t="str">
-        <v>07:30</v>
+        <v>10:00</v>
       </c>
       <c r="K89" t="str">
-        <v>10:00</v>
+        <v>13:20</v>
       </c>
       <c r="L89">
         <v>3</v>
@@ -5372,10 +5372,10 @@
         <v>150</v>
       </c>
       <c r="N89">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O89">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P89">
         <v>30</v>
@@ -5404,7 +5404,7 @@
         <v>EMH</v>
       </c>
       <c r="F90" t="str">
-        <v>G2-R2</v>
+        <v>G2-R6</v>
       </c>
       <c r="G90" t="str">
         <v>Non-Lab</v>
@@ -5413,13 +5413,13 @@
         <v>No</v>
       </c>
       <c r="I90" t="str">
-        <v>Wednesday</v>
+        <v>Friday</v>
       </c>
       <c r="J90" t="str">
-        <v>10:00</v>
+        <v>15:30</v>
       </c>
       <c r="K90" t="str">
-        <v>13:20</v>
+        <v>18:00</v>
       </c>
       <c r="L90">
         <v>3</v>
@@ -5428,10 +5428,10 @@
         <v>150</v>
       </c>
       <c r="N90">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O90">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P90">
         <v>30</v>
@@ -5460,7 +5460,7 @@
         <v>NWF</v>
       </c>
       <c r="F91" t="str">
-        <v>G4-R3</v>
+        <v>CM-202</v>
       </c>
       <c r="G91" t="str">
         <v>Non-Lab</v>
@@ -5469,13 +5469,13 @@
         <v>No</v>
       </c>
       <c r="I91" t="str">
-        <v>Friday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J91" t="str">
-        <v>07:30</v>
+        <v>08:20</v>
       </c>
       <c r="K91" t="str">
-        <v>09:10</v>
+        <v>10:00</v>
       </c>
       <c r="L91">
         <v>2</v>
@@ -5516,7 +5516,7 @@
         <v>NWF</v>
       </c>
       <c r="F92" t="str">
-        <v>CM-103</v>
+        <v>CM-202</v>
       </c>
       <c r="G92" t="str">
         <v>Non-Lab</v>
@@ -5525,13 +5525,13 @@
         <v>No</v>
       </c>
       <c r="I92" t="str">
-        <v>Monday</v>
+        <v>Thursday</v>
       </c>
       <c r="J92" t="str">
-        <v>10:00</v>
+        <v>07:30</v>
       </c>
       <c r="K92" t="str">
-        <v>11:40</v>
+        <v>09:10</v>
       </c>
       <c r="L92">
         <v>2</v>
@@ -5572,7 +5572,7 @@
         <v>AHD</v>
       </c>
       <c r="F93" t="str">
-        <v>CM-103</v>
+        <v>CM-205</v>
       </c>
       <c r="G93" t="str">
         <v>Non-Lab</v>
@@ -5581,13 +5581,13 @@
         <v>No</v>
       </c>
       <c r="I93" t="str">
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="J93" t="str">
-        <v>16:20</v>
+        <v>09:10</v>
       </c>
       <c r="K93" t="str">
-        <v>18:00</v>
+        <v>10:50</v>
       </c>
       <c r="L93">
         <v>2</v>
@@ -5637,7 +5637,7 @@
         <v>No</v>
       </c>
       <c r="I94" t="str">
-        <v>Wednesday</v>
+        <v>Monday</v>
       </c>
       <c r="J94" t="str">
         <v>13:20</v>
@@ -5684,7 +5684,7 @@
         <v>AAV</v>
       </c>
       <c r="F95" t="str">
-        <v>G2-R5</v>
+        <v>G3-R1</v>
       </c>
       <c r="G95" t="str">
         <v>Non-Lab</v>
@@ -5696,10 +5696,10 @@
         <v>Thursday</v>
       </c>
       <c r="J95" t="str">
-        <v>10:00</v>
+        <v>12:30</v>
       </c>
       <c r="K95" t="str">
-        <v>11:40</v>
+        <v>14:10</v>
       </c>
       <c r="L95">
         <v>2</v>
@@ -5740,7 +5740,7 @@
         <v>AEP</v>
       </c>
       <c r="F96" t="str">
-        <v>G2-R2</v>
+        <v>G2-R4</v>
       </c>
       <c r="G96" t="str">
         <v>Non-Lab</v>
@@ -5752,10 +5752,10 @@
         <v>Monday</v>
       </c>
       <c r="J96" t="str">
-        <v>15:30</v>
+        <v>07:30</v>
       </c>
       <c r="K96" t="str">
-        <v>18:00</v>
+        <v>10:00</v>
       </c>
       <c r="L96">
         <v>3</v>
@@ -5796,7 +5796,7 @@
         <v>AEP</v>
       </c>
       <c r="F97" t="str">
-        <v>G2-R7</v>
+        <v>G3-R1</v>
       </c>
       <c r="G97" t="str">
         <v>Non-Lab</v>
@@ -5808,10 +5808,10 @@
         <v>Friday</v>
       </c>
       <c r="J97" t="str">
-        <v>09:10</v>
+        <v>10:00</v>
       </c>
       <c r="K97" t="str">
-        <v>11:40</v>
+        <v>13:20</v>
       </c>
       <c r="L97">
         <v>3</v>
@@ -5820,10 +5820,10 @@
         <v>150</v>
       </c>
       <c r="N97">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O97">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P97">
         <v>15</v>
@@ -5852,7 +5852,7 @@
         <v>CWR</v>
       </c>
       <c r="F98" t="str">
-        <v>G4-R3</v>
+        <v>CM-101</v>
       </c>
       <c r="G98" t="str">
         <v>Non-Lab</v>
@@ -5908,7 +5908,7 @@
         <v>YNK</v>
       </c>
       <c r="F99" t="str">
-        <v>CM-202</v>
+        <v>CM-204</v>
       </c>
       <c r="G99" t="str">
         <v>Non-Lab</v>
@@ -5917,7 +5917,7 @@
         <v>No</v>
       </c>
       <c r="I99" t="str">
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="J99" t="str">
         <v>07:30</v>
@@ -5964,7 +5964,7 @@
         <v>NCS</v>
       </c>
       <c r="F100" t="str">
-        <v>G4-R3</v>
+        <v>CM-202</v>
       </c>
       <c r="G100" t="str">
         <v>Non-Lab</v>
@@ -6020,7 +6020,7 @@
         <v>CWR</v>
       </c>
       <c r="F101" t="str">
-        <v>CM-205</v>
+        <v>G4-R1</v>
       </c>
       <c r="G101" t="str">
         <v>Non-Lab</v>
@@ -6076,7 +6076,7 @@
         <v>AHD</v>
       </c>
       <c r="F102" t="str">
-        <v>G4-R2</v>
+        <v>CM-102</v>
       </c>
       <c r="G102" t="str">
         <v>Non-Lab</v>
@@ -6088,10 +6088,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J102" t="str">
-        <v>07:30</v>
+        <v>13:20</v>
       </c>
       <c r="K102" t="str">
-        <v>09:10</v>
+        <v>15:00</v>
       </c>
       <c r="L102">
         <v>2</v>
@@ -6132,7 +6132,7 @@
         <v>CWR</v>
       </c>
       <c r="F103" t="str">
-        <v>G4-R1</v>
+        <v>CM-102</v>
       </c>
       <c r="G103" t="str">
         <v>Non-Lab</v>
@@ -6188,7 +6188,7 @@
         <v>PMN</v>
       </c>
       <c r="F104" t="str">
-        <v>G4-R3</v>
+        <v>CM-102</v>
       </c>
       <c r="G104" t="str">
         <v>Non-Lab</v>
@@ -6197,13 +6197,13 @@
         <v>No</v>
       </c>
       <c r="I104" t="str">
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J104" t="str">
-        <v>07:30</v>
+        <v>10:50</v>
       </c>
       <c r="K104" t="str">
-        <v>09:10</v>
+        <v>13:20</v>
       </c>
       <c r="L104">
         <v>2</v>
@@ -6212,10 +6212,10 @@
         <v>100</v>
       </c>
       <c r="N104">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O104">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="P104">
         <v>35</v>
@@ -6256,10 +6256,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J105" t="str">
-        <v>13:20</v>
+        <v>07:30</v>
       </c>
       <c r="K105" t="str">
-        <v>15:00</v>
+        <v>09:10</v>
       </c>
       <c r="L105">
         <v>2</v>
@@ -6300,7 +6300,7 @@
         <v>MMP</v>
       </c>
       <c r="F106" t="str">
-        <v>CM-Lab3</v>
+        <v>CM-207</v>
       </c>
       <c r="G106" t="str">
         <v>Lab</v>
@@ -6309,13 +6309,13 @@
         <v>No</v>
       </c>
       <c r="I106" t="str">
-        <v>Tuesday</v>
+        <v>Friday</v>
       </c>
       <c r="J106" t="str">
+        <v>14:10</v>
+      </c>
+      <c r="K106" t="str">
         <v>16:20</v>
-      </c>
-      <c r="K106" t="str">
-        <v>18:00</v>
       </c>
       <c r="L106">
         <v>2</v>
@@ -6324,10 +6324,10 @@
         <v>100</v>
       </c>
       <c r="N106">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O106">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P106">
         <v>35</v>
@@ -6356,7 +6356,7 @@
         <v>MMP</v>
       </c>
       <c r="F107" t="str">
-        <v>CM-206</v>
+        <v>CM-207</v>
       </c>
       <c r="G107" t="str">
         <v>Lab</v>
@@ -6365,13 +6365,13 @@
         <v>No</v>
       </c>
       <c r="I107" t="str">
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J107" t="str">
-        <v>16:20</v>
+        <v>08:20</v>
       </c>
       <c r="K107" t="str">
-        <v>18:00</v>
+        <v>10:00</v>
       </c>
       <c r="L107">
         <v>2</v>
@@ -6412,7 +6412,7 @@
         <v>NWF</v>
       </c>
       <c r="F108" t="str">
-        <v>CM-102</v>
+        <v>G4-R2</v>
       </c>
       <c r="G108" t="str">
         <v>Non-Lab</v>
@@ -6421,13 +6421,13 @@
         <v>No</v>
       </c>
       <c r="I108" t="str">
-        <v>Wednesday</v>
+        <v>Friday</v>
       </c>
       <c r="J108" t="str">
-        <v>09:10</v>
+        <v>08:20</v>
       </c>
       <c r="K108" t="str">
-        <v>10:50</v>
+        <v>10:00</v>
       </c>
       <c r="L108">
         <v>2</v>
@@ -6477,13 +6477,13 @@
         <v>No</v>
       </c>
       <c r="I109" t="str">
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J109" t="str">
-        <v>16:20</v>
+        <v>10:00</v>
       </c>
       <c r="K109" t="str">
-        <v>18:00</v>
+        <v>11:40</v>
       </c>
       <c r="L109">
         <v>2</v>
@@ -6524,7 +6524,7 @@
         <v>ARI</v>
       </c>
       <c r="F110" t="str">
-        <v>G4-R3</v>
+        <v>G4-R2</v>
       </c>
       <c r="G110" t="str">
         <v>Non-Lab</v>
@@ -6533,13 +6533,13 @@
         <v>No</v>
       </c>
       <c r="I110" t="str">
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J110" t="str">
-        <v>14:10</v>
+        <v>13:20</v>
       </c>
       <c r="K110" t="str">
-        <v>16:20</v>
+        <v>15:00</v>
       </c>
       <c r="L110">
         <v>2</v>
@@ -6548,10 +6548,10 @@
         <v>100</v>
       </c>
       <c r="N110">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O110">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="P110">
         <v>60</v>
@@ -6580,7 +6580,7 @@
         <v>UAG</v>
       </c>
       <c r="F111" t="str">
-        <v>G4-R2</v>
+        <v>G4-R3</v>
       </c>
       <c r="G111" t="str">
         <v>Non-Lab</v>
@@ -6589,13 +6589,13 @@
         <v>No</v>
       </c>
       <c r="I111" t="str">
-        <v>Wednesday</v>
+        <v>Friday</v>
       </c>
       <c r="J111" t="str">
-        <v>16:20</v>
+        <v>10:00</v>
       </c>
       <c r="K111" t="str">
-        <v>19:20</v>
+        <v>13:20</v>
       </c>
       <c r="L111">
         <v>3</v>
@@ -6604,10 +6604,10 @@
         <v>150</v>
       </c>
       <c r="N111">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O111">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="P111">
         <v>52</v>
@@ -6636,7 +6636,7 @@
         <v>UAG</v>
       </c>
       <c r="F112" t="str">
-        <v>G4-R2</v>
+        <v>G4-R4</v>
       </c>
       <c r="G112" t="str">
         <v>Non-Lab</v>
@@ -6645,13 +6645,13 @@
         <v>No</v>
       </c>
       <c r="I112" t="str">
-        <v>Thursday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J112" t="str">
-        <v>07:30</v>
+        <v>15:30</v>
       </c>
       <c r="K112" t="str">
-        <v>10:00</v>
+        <v>18:00</v>
       </c>
       <c r="L112">
         <v>3</v>
@@ -6692,7 +6692,7 @@
         <v>WKS</v>
       </c>
       <c r="F113" t="str">
-        <v>G4-R3</v>
+        <v>CM-101</v>
       </c>
       <c r="G113" t="str">
         <v>Non-Lab</v>
@@ -6748,7 +6748,7 @@
         <v>PMN</v>
       </c>
       <c r="F114" t="str">
-        <v>G4-R3</v>
+        <v>CM-208</v>
       </c>
       <c r="G114" t="str">
         <v>Non-Lab</v>
@@ -6757,7 +6757,7 @@
         <v>No</v>
       </c>
       <c r="I114" t="str">
-        <v>Thursday</v>
+        <v>Monday</v>
       </c>
       <c r="J114" t="str">
         <v>10:00</v>
@@ -6804,7 +6804,7 @@
         <v>PMN</v>
       </c>
       <c r="F115" t="str">
-        <v>CM-208</v>
+        <v>G4-R4</v>
       </c>
       <c r="G115" t="str">
         <v>Non-Lab</v>
@@ -6813,13 +6813,13 @@
         <v>No</v>
       </c>
       <c r="I115" t="str">
-        <v>Tuesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J115" t="str">
-        <v>10:50</v>
+        <v>10:00</v>
       </c>
       <c r="K115" t="str">
-        <v>13:20</v>
+        <v>11:40</v>
       </c>
       <c r="L115">
         <v>2</v>
@@ -6828,10 +6828,10 @@
         <v>100</v>
       </c>
       <c r="N115">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O115">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P115">
         <v>45</v>
@@ -6860,7 +6860,7 @@
         <v>PMN</v>
       </c>
       <c r="F116" t="str">
-        <v>G4-R3</v>
+        <v>CM-204</v>
       </c>
       <c r="G116" t="str">
         <v>Non-Lab</v>
@@ -6869,13 +6869,13 @@
         <v>No</v>
       </c>
       <c r="I116" t="str">
-        <v>Monday</v>
+        <v>Thursday</v>
       </c>
       <c r="J116" t="str">
-        <v>10:00</v>
+        <v>16:20</v>
       </c>
       <c r="K116" t="str">
-        <v>11:40</v>
+        <v>18:00</v>
       </c>
       <c r="L116">
         <v>2</v>
@@ -6925,13 +6925,13 @@
         <v>No</v>
       </c>
       <c r="I117" t="str">
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J117" t="str">
-        <v>10:50</v>
+        <v>16:20</v>
       </c>
       <c r="K117" t="str">
-        <v>14:10</v>
+        <v>19:20</v>
       </c>
       <c r="L117">
         <v>3</v>
@@ -6940,10 +6940,10 @@
         <v>150</v>
       </c>
       <c r="N117">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="O117">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="P117">
         <v>45</v>
@@ -6972,7 +6972,7 @@
         <v>WND</v>
       </c>
       <c r="F118" t="str">
-        <v>CM-208</v>
+        <v>G4-R3</v>
       </c>
       <c r="G118" t="str">
         <v>Non-Lab</v>
@@ -6981,13 +6981,13 @@
         <v>No</v>
       </c>
       <c r="I118" t="str">
-        <v>Wednesday</v>
+        <v>Friday</v>
       </c>
       <c r="J118" t="str">
-        <v>13:20</v>
+        <v>16:20</v>
       </c>
       <c r="K118" t="str">
-        <v>16:20</v>
+        <v>19:20</v>
       </c>
       <c r="L118">
         <v>3</v>
@@ -7084,7 +7084,7 @@
         <v>FAP</v>
       </c>
       <c r="F120" t="str">
-        <v>G4-R1</v>
+        <v>G4-R4</v>
       </c>
       <c r="G120" t="str">
         <v>Non-Lab</v>
@@ -7093,13 +7093,13 @@
         <v>No</v>
       </c>
       <c r="I120" t="str">
-        <v>Thursday</v>
+        <v>Monday</v>
       </c>
       <c r="J120" t="str">
-        <v>12:30</v>
+        <v>10:00</v>
       </c>
       <c r="K120" t="str">
-        <v>14:10</v>
+        <v>11:40</v>
       </c>
       <c r="L120">
         <v>2</v>
@@ -7145,7 +7145,7 @@
         <v>MHA</v>
       </c>
       <c r="F121" t="str">
-        <v>G4-R1</v>
+        <v>G4-R3</v>
       </c>
       <c r="G121" t="str">
         <v>Non-Lab</v>
@@ -7157,10 +7157,10 @@
         <v>Monday</v>
       </c>
       <c r="J121" t="str">
-        <v>13:20</v>
+        <v>12:30</v>
       </c>
       <c r="K121" t="str">
-        <v>15:00</v>
+        <v>14:10</v>
       </c>
       <c r="L121">
         <v>2</v>
@@ -7201,7 +7201,7 @@
         <v>SII, CWR</v>
       </c>
       <c r="F122" t="str">
-        <v>G4-R2</v>
+        <v>G4-R4</v>
       </c>
       <c r="G122" t="str">
         <v>Non-Lab</v>
@@ -7210,13 +7210,13 @@
         <v>No</v>
       </c>
       <c r="I122" t="str">
-        <v>Tuesday</v>
+        <v>Monday</v>
       </c>
       <c r="J122" t="str">
-        <v>13:20</v>
+        <v>16:20</v>
       </c>
       <c r="K122" t="str">
-        <v>16:20</v>
+        <v>19:20</v>
       </c>
       <c r="L122">
         <v>3</v>
@@ -7257,7 +7257,7 @@
         <v>UAG</v>
       </c>
       <c r="F123" t="str">
-        <v>G4-R1</v>
+        <v>G4-R4</v>
       </c>
       <c r="G123" t="str">
         <v>Non-Lab</v>
@@ -7269,10 +7269,10 @@
         <v>Monday</v>
       </c>
       <c r="J123" t="str">
-        <v>10:00</v>
+        <v>14:10</v>
       </c>
       <c r="K123" t="str">
-        <v>11:40</v>
+        <v>16:20</v>
       </c>
       <c r="L123">
         <v>2</v>
@@ -7281,10 +7281,10 @@
         <v>100</v>
       </c>
       <c r="N123">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O123">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P123">
         <v>50</v>
@@ -7313,7 +7313,7 @@
         <v>FAP</v>
       </c>
       <c r="F124" t="str">
-        <v>G4-R2</v>
+        <v>G4-R1</v>
       </c>
       <c r="G124" t="str">
         <v>Non-Lab</v>
@@ -7322,13 +7322,13 @@
         <v>No</v>
       </c>
       <c r="I124" t="str">
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J124" t="str">
-        <v>12:30</v>
+        <v>15:30</v>
       </c>
       <c r="K124" t="str">
-        <v>13:20</v>
+        <v>16:20</v>
       </c>
       <c r="L124">
         <v>1</v>
@@ -7425,7 +7425,7 @@
         <v>SII, CWR</v>
       </c>
       <c r="F126" t="str">
-        <v>G4-R4</v>
+        <v>G4-R1</v>
       </c>
       <c r="G126" t="str">
         <v>Non-Lab</v>
@@ -7493,10 +7493,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J127" t="str">
-        <v>16:20</v>
+        <v>13:20</v>
       </c>
       <c r="K127" t="str">
-        <v>18:00</v>
+        <v>15:00</v>
       </c>
       <c r="L127">
         <v>2</v>
@@ -7537,7 +7537,7 @@
         <v>FAP</v>
       </c>
       <c r="F128" t="str">
-        <v>G2-R2</v>
+        <v>G2-R5</v>
       </c>
       <c r="G128" t="str">
         <v>Non-Lab</v>
@@ -7546,13 +7546,13 @@
         <v>No</v>
       </c>
       <c r="I128" t="str">
-        <v>Thursday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J128" t="str">
-        <v>14:10</v>
+        <v>16:20</v>
       </c>
       <c r="K128" t="str">
-        <v>16:20</v>
+        <v>18:00</v>
       </c>
       <c r="L128">
         <v>2</v>
@@ -7561,10 +7561,10 @@
         <v>100</v>
       </c>
       <c r="N128">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O128">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="P128">
         <v>30</v>
@@ -7593,7 +7593,7 @@
         <v>FAP</v>
       </c>
       <c r="F129" t="str">
-        <v>G2-R3</v>
+        <v>B3-R1</v>
       </c>
       <c r="G129" t="str">
         <v>Non-Lab</v>
@@ -7602,13 +7602,13 @@
         <v>No</v>
       </c>
       <c r="I129" t="str">
-        <v>Monday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J129" t="str">
-        <v>12:30</v>
+        <v>09:10</v>
       </c>
       <c r="K129" t="str">
-        <v>13:20</v>
+        <v>10:00</v>
       </c>
       <c r="L129">
         <v>1</v>
@@ -7649,7 +7649,7 @@
         <v>SII</v>
       </c>
       <c r="F130" t="str">
-        <v>G2-R6</v>
+        <v>G2-R4</v>
       </c>
       <c r="G130" t="str">
         <v>Non-Lab</v>
@@ -7661,10 +7661,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J130" t="str">
-        <v>09:10</v>
+        <v>10:00</v>
       </c>
       <c r="K130" t="str">
-        <v>10:00</v>
+        <v>10:50</v>
       </c>
       <c r="L130">
         <v>1</v>
@@ -7705,7 +7705,7 @@
         <v>UAG</v>
       </c>
       <c r="F131" t="str">
-        <v>G2-R4</v>
+        <v>CM-204</v>
       </c>
       <c r="G131" t="str">
         <v>Non-Lab</v>
@@ -7714,13 +7714,13 @@
         <v>No</v>
       </c>
       <c r="I131" t="str">
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J131" t="str">
-        <v>14:10</v>
+        <v>07:30</v>
       </c>
       <c r="K131" t="str">
-        <v>16:20</v>
+        <v>09:10</v>
       </c>
       <c r="L131">
         <v>2</v>
@@ -7729,10 +7729,10 @@
         <v>100</v>
       </c>
       <c r="N131">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O131">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="P131">
         <v>30</v>
@@ -7761,7 +7761,7 @@
         <v>YNK</v>
       </c>
       <c r="F132" t="str">
-        <v>G4-R4</v>
+        <v>CM-205</v>
       </c>
       <c r="G132" t="str">
         <v>Non-Lab</v>
@@ -7817,7 +7817,7 @@
         <v>YNK</v>
       </c>
       <c r="F133" t="str">
-        <v>G3-R2</v>
+        <v>G2-R2</v>
       </c>
       <c r="G133" t="str">
         <v>Non-Lab</v>
@@ -7873,7 +7873,7 @@
         <v>UAG</v>
       </c>
       <c r="F134" t="str">
-        <v>G2-R5</v>
+        <v>B3-R2</v>
       </c>
       <c r="G134" t="str">
         <v>Non-Lab</v>
@@ -7882,13 +7882,13 @@
         <v>No</v>
       </c>
       <c r="I134" t="str">
-        <v>Monday</v>
+        <v>Thursday</v>
       </c>
       <c r="J134" t="str">
-        <v>15:30</v>
+        <v>10:00</v>
       </c>
       <c r="K134" t="str">
-        <v>17:10</v>
+        <v>11:40</v>
       </c>
       <c r="L134">
         <v>2</v>
@@ -7929,7 +7929,7 @@
         <v>UAG</v>
       </c>
       <c r="F135" t="str">
-        <v>B2-R1</v>
+        <v>G4-R2</v>
       </c>
       <c r="G135" t="str">
         <v>Non-Lab</v>
@@ -7938,13 +7938,13 @@
         <v>No</v>
       </c>
       <c r="I135" t="str">
-        <v>Thursday</v>
+        <v>Friday</v>
       </c>
       <c r="J135" t="str">
-        <v>10:00</v>
+        <v>14:10</v>
       </c>
       <c r="K135" t="str">
-        <v>11:40</v>
+        <v>16:20</v>
       </c>
       <c r="L135">
         <v>2</v>
@@ -7953,10 +7953,10 @@
         <v>100</v>
       </c>
       <c r="N135">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O135">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P135">
         <v>30</v>
@@ -7985,7 +7985,7 @@
         <v>ARH</v>
       </c>
       <c r="F136" t="str">
-        <v>G4-R4</v>
+        <v>CM-205</v>
       </c>
       <c r="G136" t="str">
         <v>Non-Lab</v>
@@ -7997,10 +7997,10 @@
         <v>Wednesday</v>
       </c>
       <c r="J136" t="str">
-        <v>15:30</v>
+        <v>16:20</v>
       </c>
       <c r="K136" t="str">
-        <v>17:10</v>
+        <v>18:00</v>
       </c>
       <c r="L136">
         <v>2</v>
@@ -8041,7 +8041,7 @@
         <v>UAG, FAP</v>
       </c>
       <c r="F137" t="str">
-        <v>G2-R7</v>
+        <v>CM-201</v>
       </c>
       <c r="G137" t="str">
         <v>Non-Lab</v>
@@ -8050,13 +8050,13 @@
         <v>No</v>
       </c>
       <c r="I137" t="str">
-        <v>Wednesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J137" t="str">
-        <v>07:30</v>
+        <v>13:20</v>
       </c>
       <c r="K137" t="str">
-        <v>09:10</v>
+        <v>15:00</v>
       </c>
       <c r="L137">
         <v>2</v>
@@ -8097,7 +8097,7 @@
         <v>ARI</v>
       </c>
       <c r="F138" t="str">
-        <v>G4-R3</v>
+        <v>G4-R2</v>
       </c>
       <c r="G138" t="str">
         <v>Non-Lab</v>
@@ -8165,10 +8165,10 @@
         <v>Thursday</v>
       </c>
       <c r="J139" t="str">
-        <v>16:20</v>
+        <v>15:30</v>
       </c>
       <c r="K139" t="str">
-        <v>19:20</v>
+        <v>18:00</v>
       </c>
       <c r="L139">
         <v>3</v>
@@ -8177,10 +8177,10 @@
         <v>150</v>
       </c>
       <c r="N139">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O139">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P139">
         <v>46</v>
@@ -8210,7 +8210,7 @@
         <v>FAP, ARH</v>
       </c>
       <c r="F140" t="str">
-        <v>G4-R2</v>
+        <v>G4-R1</v>
       </c>
       <c r="G140" t="str">
         <v>Non-Lab</v>
@@ -8266,7 +8266,7 @@
         <v>SII, YNK</v>
       </c>
       <c r="F141" t="str">
-        <v>G4-R3</v>
+        <v>G4-R1</v>
       </c>
       <c r="G141" t="str">
         <v>Non-Lab</v>
@@ -8378,7 +8378,7 @@
         <v>FAP</v>
       </c>
       <c r="F143" t="str">
-        <v>G2-R6</v>
+        <v>G3-R4</v>
       </c>
       <c r="G143" t="str">
         <v>Non-Lab</v>
@@ -8390,10 +8390,10 @@
         <v>Monday</v>
       </c>
       <c r="J143" t="str">
-        <v>07:30</v>
+        <v>16:20</v>
       </c>
       <c r="K143" t="str">
-        <v>10:00</v>
+        <v>19:20</v>
       </c>
       <c r="L143">
         <v>3</v>
@@ -8402,10 +8402,10 @@
         <v>150</v>
       </c>
       <c r="N143">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O143">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="P143">
         <v>30</v>
@@ -8434,7 +8434,7 @@
         <v>YNK</v>
       </c>
       <c r="F144" t="str">
-        <v>CM-102</v>
+        <v>CM-201</v>
       </c>
       <c r="G144" t="str">
         <v>Non-Lab</v>
@@ -8490,7 +8490,7 @@
         <v>YSM, WKS</v>
       </c>
       <c r="F145" t="str">
-        <v>B3-R1</v>
+        <v>G2-R2</v>
       </c>
       <c r="G145" t="str">
         <v>Non-Lab</v>
@@ -8499,13 +8499,13 @@
         <v>No</v>
       </c>
       <c r="I145" t="str">
-        <v>Wednesday</v>
+        <v>Monday</v>
       </c>
       <c r="J145" t="str">
-        <v>07:30</v>
+        <v>10:00</v>
       </c>
       <c r="K145" t="str">
-        <v>10:00</v>
+        <v>13:20</v>
       </c>
       <c r="L145">
         <v>3</v>
@@ -8514,10 +8514,10 @@
         <v>150</v>
       </c>
       <c r="N145">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O145">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P145">
         <v>30</v>
@@ -8546,7 +8546,7 @@
         <v>YSM, WKS</v>
       </c>
       <c r="F146" t="str">
-        <v>CM-204</v>
+        <v>G2-R7</v>
       </c>
       <c r="G146" t="str">
         <v>Non-Lab</v>
@@ -8555,13 +8555,13 @@
         <v>No</v>
       </c>
       <c r="I146" t="str">
-        <v>Monday</v>
+        <v>Friday</v>
       </c>
       <c r="J146" t="str">
-        <v>16:20</v>
+        <v>15:30</v>
       </c>
       <c r="K146" t="str">
-        <v>19:20</v>
+        <v>18:00</v>
       </c>
       <c r="L146">
         <v>3</v>
@@ -8570,10 +8570,10 @@
         <v>150</v>
       </c>
       <c r="N146">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O146">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P146">
         <v>30</v>
@@ -8602,7 +8602,7 @@
         <v>FKH</v>
       </c>
       <c r="F147" t="str">
-        <v>B3-R2</v>
+        <v>CM-205</v>
       </c>
       <c r="G147" t="str">
         <v>Non-Lab</v>
@@ -8614,10 +8614,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J147" t="str">
-        <v>16:20</v>
+        <v>13:20</v>
       </c>
       <c r="K147" t="str">
-        <v>18:00</v>
+        <v>15:00</v>
       </c>
       <c r="L147">
         <v>2</v>
@@ -8658,7 +8658,7 @@
         <v>ZSR</v>
       </c>
       <c r="F148" t="str">
-        <v>G2-R4</v>
+        <v>G4-R4</v>
       </c>
       <c r="G148" t="str">
         <v>Non-Lab</v>
@@ -8670,10 +8670,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J148" t="str">
-        <v>07:30</v>
+        <v>09:10</v>
       </c>
       <c r="K148" t="str">
-        <v>09:10</v>
+        <v>10:50</v>
       </c>
       <c r="L148">
         <v>2</v>
@@ -8714,7 +8714,7 @@
         <v>FKH</v>
       </c>
       <c r="F149" t="str">
-        <v>B3-R2</v>
+        <v>G4-R4</v>
       </c>
       <c r="G149" t="str">
         <v>Non-Lab</v>
@@ -8770,7 +8770,7 @@
         <v>FKH, ZSR</v>
       </c>
       <c r="F150" t="str">
-        <v>CM-204</v>
+        <v>B3-R1</v>
       </c>
       <c r="G150" t="str">
         <v>Non-Lab</v>
@@ -8782,10 +8782,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J150" t="str">
-        <v>13:20</v>
+        <v>15:30</v>
       </c>
       <c r="K150" t="str">
-        <v>16:20</v>
+        <v>18:00</v>
       </c>
       <c r="L150">
         <v>3</v>
@@ -8794,10 +8794,10 @@
         <v>150</v>
       </c>
       <c r="N150">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O150">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P150">
         <v>30</v>
@@ -8826,7 +8826,7 @@
         <v>FKH, ZSR</v>
       </c>
       <c r="F151" t="str">
-        <v>CM-203</v>
+        <v>G2-R5</v>
       </c>
       <c r="G151" t="str">
         <v>Non-Lab</v>
@@ -8835,13 +8835,13 @@
         <v>No</v>
       </c>
       <c r="I151" t="str">
-        <v>Wednesday</v>
+        <v>Friday</v>
       </c>
       <c r="J151" t="str">
-        <v>13:20</v>
+        <v>10:50</v>
       </c>
       <c r="K151" t="str">
-        <v>16:20</v>
+        <v>14:10</v>
       </c>
       <c r="L151">
         <v>3</v>
@@ -8850,10 +8850,10 @@
         <v>150</v>
       </c>
       <c r="N151">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O151">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="P151">
         <v>30</v>
@@ -8882,7 +8882,7 @@
         <v>YSM, WKS</v>
       </c>
       <c r="F152" t="str">
-        <v>G2-R5</v>
+        <v>G4-R4</v>
       </c>
       <c r="G152" t="str">
         <v>Non-Lab</v>
@@ -8891,14 +8891,14 @@
         <v>No</v>
       </c>
       <c r="I152" t="str">
-        <v>Monday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J152" t="str">
+        <v>07:30</v>
+      </c>
+      <c r="K152" t="str">
         <v>10:00</v>
       </c>
-      <c r="K152" t="str">
-        <v>13:20</v>
-      </c>
       <c r="L152">
         <v>3</v>
       </c>
@@ -8906,10 +8906,10 @@
         <v>150</v>
       </c>
       <c r="N152">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O152">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P152">
         <v>30</v>
@@ -8938,7 +8938,7 @@
         <v>WKS</v>
       </c>
       <c r="F153" t="str">
-        <v>G2-R5</v>
+        <v>CM-205</v>
       </c>
       <c r="G153" t="str">
         <v>Non-Lab</v>
@@ -8947,13 +8947,13 @@
         <v>No</v>
       </c>
       <c r="I153" t="str">
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J153" t="str">
-        <v>15:30</v>
+        <v>12:30</v>
       </c>
       <c r="K153" t="str">
-        <v>18:00</v>
+        <v>15:00</v>
       </c>
       <c r="L153">
         <v>3</v>
@@ -8994,7 +8994,7 @@
         <v>YSM</v>
       </c>
       <c r="F154" t="str">
-        <v>G3-R4</v>
+        <v>G2-R2</v>
       </c>
       <c r="G154" t="str">
         <v>Non-Lab</v>
@@ -9003,13 +9003,13 @@
         <v>No</v>
       </c>
       <c r="I154" t="str">
-        <v>Wednesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J154" t="str">
-        <v>10:00</v>
+        <v>13:20</v>
       </c>
       <c r="K154" t="str">
-        <v>13:20</v>
+        <v>16:20</v>
       </c>
       <c r="L154">
         <v>3</v>
@@ -9018,10 +9018,10 @@
         <v>150</v>
       </c>
       <c r="N154">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="O154">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="P154">
         <v>30</v>
@@ -9050,7 +9050,7 @@
         <v>YSM, WKS</v>
       </c>
       <c r="F155" t="str">
-        <v>CM-204</v>
+        <v>CM-201</v>
       </c>
       <c r="G155" t="str">
         <v>Non-Lab</v>
@@ -9062,10 +9062,10 @@
         <v>Wednesday</v>
       </c>
       <c r="J155" t="str">
-        <v>16:20</v>
+        <v>10:00</v>
       </c>
       <c r="K155" t="str">
-        <v>18:00</v>
+        <v>11:40</v>
       </c>
       <c r="L155">
         <v>2</v>
@@ -9106,7 +9106,7 @@
         <v>FKH, ZSR</v>
       </c>
       <c r="F156" t="str">
-        <v>G3-R1</v>
+        <v>G4-R4</v>
       </c>
       <c r="G156" t="str">
         <v>Non-Lab</v>
@@ -9162,7 +9162,7 @@
         <v>YSM, WKS</v>
       </c>
       <c r="F157" t="str">
-        <v>G4-R3</v>
+        <v>G2-R4</v>
       </c>
       <c r="G157" t="str">
         <v>Non-Lab</v>
@@ -9171,13 +9171,13 @@
         <v>No</v>
       </c>
       <c r="I157" t="str">
-        <v>Tuesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J157" t="str">
-        <v>09:10</v>
+        <v>16:20</v>
       </c>
       <c r="K157" t="str">
-        <v>10:50</v>
+        <v>18:00</v>
       </c>
       <c r="L157">
         <v>2</v>
@@ -9218,7 +9218,7 @@
         <v>FKH, YSM</v>
       </c>
       <c r="F158" t="str">
-        <v>CM-103</v>
+        <v>G2-R4</v>
       </c>
       <c r="G158" t="str">
         <v>Non-Lab</v>
@@ -9227,13 +9227,13 @@
         <v>No</v>
       </c>
       <c r="I158" t="str">
-        <v>Thursday</v>
+        <v>Friday</v>
       </c>
       <c r="J158" t="str">
-        <v>10:00</v>
+        <v>07:30</v>
       </c>
       <c r="K158" t="str">
-        <v>11:40</v>
+        <v>09:10</v>
       </c>
       <c r="L158">
         <v>2</v>
@@ -9274,7 +9274,7 @@
         <v>ZSR, FKH</v>
       </c>
       <c r="F159" t="str">
-        <v>G2-R3</v>
+        <v>G4-R1</v>
       </c>
       <c r="G159" t="str">
         <v>Non-Lab</v>
@@ -9286,10 +9286,10 @@
         <v>Thursday</v>
       </c>
       <c r="J159" t="str">
-        <v>12:30</v>
+        <v>10:00</v>
       </c>
       <c r="K159" t="str">
-        <v>15:00</v>
+        <v>13:20</v>
       </c>
       <c r="L159">
         <v>3</v>
@@ -9298,10 +9298,10 @@
         <v>150</v>
       </c>
       <c r="N159">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O159">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P159">
         <v>30</v>
@@ -9330,7 +9330,7 @@
         <v>ZSR</v>
       </c>
       <c r="F160" t="str">
-        <v>B3-R2</v>
+        <v>CM-102</v>
       </c>
       <c r="G160" t="str">
         <v>Non-Lab</v>
@@ -9339,7 +9339,7 @@
         <v>No</v>
       </c>
       <c r="I160" t="str">
-        <v>Friday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J160" t="str">
         <v>07:30</v>
@@ -9386,7 +9386,7 @@
         <v>FKH</v>
       </c>
       <c r="F161" t="str">
-        <v>G2-R4</v>
+        <v>G3-R2</v>
       </c>
       <c r="G161" t="str">
         <v>Non-Lab</v>
@@ -9395,13 +9395,13 @@
         <v>No</v>
       </c>
       <c r="I161" t="str">
-        <v>Friday</v>
+        <v>Monday</v>
       </c>
       <c r="J161" t="str">
-        <v>09:10</v>
+        <v>07:30</v>
       </c>
       <c r="K161" t="str">
-        <v>11:40</v>
+        <v>10:00</v>
       </c>
       <c r="L161">
         <v>3</v>
@@ -9442,7 +9442,7 @@
         <v>YSM</v>
       </c>
       <c r="F162" t="str">
-        <v>G2-R5</v>
+        <v>G3-R2</v>
       </c>
       <c r="G162" t="str">
         <v>Non-Lab</v>
@@ -9451,7 +9451,7 @@
         <v>No</v>
       </c>
       <c r="I162" t="str">
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J162" t="str">
         <v>15:30</v>
@@ -9498,7 +9498,7 @@
         <v>NGT</v>
       </c>
       <c r="F163" t="str">
-        <v>G4-R3</v>
+        <v>B3-R2</v>
       </c>
       <c r="G163" t="str">
         <v>Non-Lab</v>
@@ -9507,13 +9507,13 @@
         <v>No</v>
       </c>
       <c r="I163" t="str">
-        <v>Wednesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J163" t="str">
-        <v>09:10</v>
+        <v>15:30</v>
       </c>
       <c r="K163" t="str">
-        <v>11:40</v>
+        <v>18:00</v>
       </c>
       <c r="L163">
         <v>3</v>
@@ -9554,7 +9554,7 @@
         <v>NGT</v>
       </c>
       <c r="F164" t="str">
-        <v>G3-R4</v>
+        <v>G4-R3</v>
       </c>
       <c r="G164" t="str">
         <v>Non-Lab</v>
@@ -9563,13 +9563,13 @@
         <v>No</v>
       </c>
       <c r="I164" t="str">
-        <v>Thursday</v>
+        <v>Friday</v>
       </c>
       <c r="J164" t="str">
-        <v>16:20</v>
+        <v>07:30</v>
       </c>
       <c r="K164" t="str">
-        <v>19:20</v>
+        <v>10:00</v>
       </c>
       <c r="L164">
         <v>3</v>
@@ -9578,10 +9578,10 @@
         <v>150</v>
       </c>
       <c r="N164">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O164">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P164">
         <v>30</v>
@@ -9610,7 +9610,7 @@
         <v>NGT, PAY</v>
       </c>
       <c r="F165" t="str">
-        <v>G3-R4</v>
+        <v>G2-R3</v>
       </c>
       <c r="G165" t="str">
         <v>Non-Lab</v>
@@ -9666,7 +9666,7 @@
         <v>NGT, PAY</v>
       </c>
       <c r="F166" t="str">
-        <v>B2-R1</v>
+        <v>CM-101</v>
       </c>
       <c r="G166" t="str">
         <v>Non-Lab</v>
@@ -9722,7 +9722,7 @@
         <v>NGT, MZF</v>
       </c>
       <c r="F167" t="str">
-        <v>G4-R3</v>
+        <v>G4-R4</v>
       </c>
       <c r="G167" t="str">
         <v>Non-Lab</v>
@@ -9731,13 +9731,13 @@
         <v>No</v>
       </c>
       <c r="I167" t="str">
-        <v>Tuesday</v>
+        <v>Friday</v>
       </c>
       <c r="J167" t="str">
-        <v>10:50</v>
+        <v>10:00</v>
       </c>
       <c r="K167" t="str">
-        <v>13:20</v>
+        <v>11:40</v>
       </c>
       <c r="L167">
         <v>2</v>
@@ -9746,10 +9746,10 @@
         <v>100</v>
       </c>
       <c r="N167">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O167">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P167">
         <v>60</v>
@@ -9778,7 +9778,7 @@
         <v>MNI</v>
       </c>
       <c r="F168" t="str">
-        <v>G5-Lab1</v>
+        <v>G5-Lab2</v>
       </c>
       <c r="G168" t="str">
         <v>Lab</v>
@@ -9834,7 +9834,7 @@
         <v>MNI</v>
       </c>
       <c r="F169" t="str">
-        <v>CM-Lab3</v>
+        <v>G5-Lab2</v>
       </c>
       <c r="G169" t="str">
         <v>Lab</v>
@@ -9890,7 +9890,7 @@
         <v>PAY</v>
       </c>
       <c r="F170" t="str">
-        <v>CM-205</v>
+        <v>CM-204</v>
       </c>
       <c r="G170" t="str">
         <v>Non-Lab</v>
@@ -9899,13 +9899,13 @@
         <v>No</v>
       </c>
       <c r="I170" t="str">
-        <v>Monday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J170" t="str">
-        <v>07:30</v>
+        <v>12:30</v>
       </c>
       <c r="K170" t="str">
-        <v>10:00</v>
+        <v>15:00</v>
       </c>
       <c r="L170">
         <v>3</v>
@@ -9946,7 +9946,7 @@
         <v>PAY</v>
       </c>
       <c r="F171" t="str">
-        <v>G2-R3</v>
+        <v>G2-R5</v>
       </c>
       <c r="G171" t="str">
         <v>Non-Lab</v>
@@ -9955,13 +9955,13 @@
         <v>No</v>
       </c>
       <c r="I171" t="str">
-        <v>Wednesday</v>
+        <v>Monday</v>
       </c>
       <c r="J171" t="str">
-        <v>15:30</v>
+        <v>10:00</v>
       </c>
       <c r="K171" t="str">
-        <v>18:00</v>
+        <v>13:20</v>
       </c>
       <c r="L171">
         <v>3</v>
@@ -9970,10 +9970,10 @@
         <v>150</v>
       </c>
       <c r="N171">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O171">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P171">
         <v>30</v>
@@ -10002,7 +10002,7 @@
         <v>MZF</v>
       </c>
       <c r="F172" t="str">
-        <v>CM-207</v>
+        <v>CM-Lab3</v>
       </c>
       <c r="G172" t="str">
         <v>Lab</v>
@@ -10058,7 +10058,7 @@
         <v>MZF</v>
       </c>
       <c r="F173" t="str">
-        <v>CM-207</v>
+        <v>CM-206</v>
       </c>
       <c r="G173" t="str">
         <v>Lab</v>
@@ -10114,7 +10114,7 @@
         <v>TQB</v>
       </c>
       <c r="F174" t="str">
-        <v>CM-LabVirtual</v>
+        <v>CM-Lab3</v>
       </c>
       <c r="G174" t="str">
         <v>Lab</v>
@@ -10123,13 +10123,13 @@
         <v>No</v>
       </c>
       <c r="I174" t="str">
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J174" t="str">
-        <v>13:20</v>
+        <v>07:30</v>
       </c>
       <c r="K174" t="str">
-        <v>16:20</v>
+        <v>10:00</v>
       </c>
       <c r="L174">
         <v>3</v>
@@ -10138,10 +10138,10 @@
         <v>150</v>
       </c>
       <c r="N174">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O174">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P174">
         <v>38</v>
@@ -10170,7 +10170,7 @@
         <v>TQB</v>
       </c>
       <c r="F175" t="str">
-        <v>CM-206</v>
+        <v>CM-207</v>
       </c>
       <c r="G175" t="str">
         <v>Lab</v>
@@ -10179,13 +10179,13 @@
         <v>No</v>
       </c>
       <c r="I175" t="str">
-        <v>Monday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J175" t="str">
-        <v>13:20</v>
+        <v>10:50</v>
       </c>
       <c r="K175" t="str">
-        <v>16:20</v>
+        <v>14:10</v>
       </c>
       <c r="L175">
         <v>3</v>
@@ -10194,10 +10194,10 @@
         <v>150</v>
       </c>
       <c r="N175">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O175">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="P175">
         <v>37</v>
@@ -10226,7 +10226,7 @@
         <v>LHY</v>
       </c>
       <c r="F176" t="str">
-        <v>G4-R4</v>
+        <v>CM-205</v>
       </c>
       <c r="G176" t="str">
         <v>Non-Lab</v>
@@ -10238,11 +10238,11 @@
         <v>Monday</v>
       </c>
       <c r="J176" t="str">
+        <v>07:30</v>
+      </c>
+      <c r="K176" t="str">
         <v>10:00</v>
       </c>
-      <c r="K176" t="str">
-        <v>13:20</v>
-      </c>
       <c r="L176">
         <v>3</v>
       </c>
@@ -10250,10 +10250,10 @@
         <v>150</v>
       </c>
       <c r="N176">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O176">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P176">
         <v>38</v>
@@ -10282,7 +10282,7 @@
         <v>LHY</v>
       </c>
       <c r="F177" t="str">
-        <v>CM-201</v>
+        <v>G4-R3</v>
       </c>
       <c r="G177" t="str">
         <v>Non-Lab</v>
@@ -10291,13 +10291,13 @@
         <v>No</v>
       </c>
       <c r="I177" t="str">
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J177" t="str">
-        <v>09:10</v>
+        <v>15:30</v>
       </c>
       <c r="K177" t="str">
-        <v>11:40</v>
+        <v>18:00</v>
       </c>
       <c r="L177">
         <v>3</v>
@@ -10338,7 +10338,7 @@
         <v>TQB</v>
       </c>
       <c r="F178" t="str">
-        <v>CM-202</v>
+        <v>G4-R2</v>
       </c>
       <c r="G178" t="str">
         <v>Non-Lab</v>
@@ -10347,13 +10347,13 @@
         <v>No</v>
       </c>
       <c r="I178" t="str">
-        <v>Wednesday</v>
+        <v>Thursday</v>
       </c>
       <c r="J178" t="str">
-        <v>12:30</v>
+        <v>13:20</v>
       </c>
       <c r="K178" t="str">
-        <v>14:10</v>
+        <v>15:00</v>
       </c>
       <c r="L178">
         <v>2</v>
@@ -10394,7 +10394,7 @@
         <v>TQB</v>
       </c>
       <c r="F179" t="str">
-        <v>CM-102</v>
+        <v>CM-101</v>
       </c>
       <c r="G179" t="str">
         <v>Non-Lab</v>
@@ -10403,13 +10403,13 @@
         <v>No</v>
       </c>
       <c r="I179" t="str">
-        <v>Wednesday</v>
+        <v>Monday</v>
       </c>
       <c r="J179" t="str">
-        <v>07:30</v>
+        <v>13:20</v>
       </c>
       <c r="K179" t="str">
-        <v>09:10</v>
+        <v>15:00</v>
       </c>
       <c r="L179">
         <v>2</v>
@@ -10450,7 +10450,7 @@
         <v>TKN</v>
       </c>
       <c r="F180" t="str">
-        <v>G4-R2</v>
+        <v>CM-201</v>
       </c>
       <c r="G180" t="str">
         <v>Non-Lab</v>
@@ -10506,7 +10506,7 @@
         <v>MAL</v>
       </c>
       <c r="F181" t="str">
-        <v>CM-202</v>
+        <v>G4-R1</v>
       </c>
       <c r="G181" t="str">
         <v>Non-Lab</v>
@@ -10562,7 +10562,7 @@
         <v>MAL</v>
       </c>
       <c r="F182" t="str">
-        <v>CM-204</v>
+        <v>CM-201</v>
       </c>
       <c r="G182" t="str">
         <v>Non-Lab</v>
@@ -10618,7 +10618,7 @@
         <v>PTA</v>
       </c>
       <c r="F183" t="str">
-        <v>CM-201</v>
+        <v>G4-R2</v>
       </c>
       <c r="G183" t="str">
         <v>Non-Lab</v>
@@ -10674,7 +10674,7 @@
         <v>PTA</v>
       </c>
       <c r="F184" t="str">
-        <v>CM-203</v>
+        <v>CM-102</v>
       </c>
       <c r="G184" t="str">
         <v>Non-Lab</v>
@@ -10730,7 +10730,7 @@
         <v>BMR</v>
       </c>
       <c r="F185" t="str">
-        <v>CM-204</v>
+        <v>G4-R2</v>
       </c>
       <c r="G185" t="str">
         <v>Non-Lab</v>
@@ -10739,13 +10739,13 @@
         <v>No</v>
       </c>
       <c r="I185" t="str">
-        <v>Thursday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J185" t="str">
-        <v>07:30</v>
+        <v>09:10</v>
       </c>
       <c r="K185" t="str">
-        <v>10:00</v>
+        <v>11:40</v>
       </c>
       <c r="L185">
         <v>3</v>
@@ -10786,7 +10786,7 @@
         <v>PTA</v>
       </c>
       <c r="F186" t="str">
-        <v>CM-202</v>
+        <v>CM-102</v>
       </c>
       <c r="G186" t="str">
         <v>Non-Lab</v>
@@ -10898,7 +10898,7 @@
         <v>ADF</v>
       </c>
       <c r="F188" t="str">
-        <v>CM-LabVirtual</v>
+        <v>CM-Lab3</v>
       </c>
       <c r="G188" t="str">
         <v>Lab</v>
@@ -10954,7 +10954,7 @@
         <v>FDN</v>
       </c>
       <c r="F189" t="str">
-        <v>CM-LabVirtual</v>
+        <v>CM-206</v>
       </c>
       <c r="G189" t="str">
         <v>Lab</v>
@@ -10963,13 +10963,13 @@
         <v>No</v>
       </c>
       <c r="I189" t="str">
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="J189" t="str">
-        <v>14:10</v>
+        <v>07:30</v>
       </c>
       <c r="K189" t="str">
-        <v>16:20</v>
+        <v>09:10</v>
       </c>
       <c r="L189">
         <v>2</v>
@@ -10978,10 +10978,10 @@
         <v>100</v>
       </c>
       <c r="N189">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O189">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="P189">
         <v>45</v>
@@ -11010,7 +11010,7 @@
         <v>FDN</v>
       </c>
       <c r="F190" t="str">
-        <v>G4-R4</v>
+        <v>CM-201</v>
       </c>
       <c r="G190" t="str">
         <v>Non-Lab</v>
@@ -11066,7 +11066,7 @@
         <v>GFP</v>
       </c>
       <c r="F191" t="str">
-        <v>CM-LabVirtual</v>
+        <v>CM-206</v>
       </c>
       <c r="G191" t="str">
         <v>Lab</v>
@@ -11075,13 +11075,13 @@
         <v>No</v>
       </c>
       <c r="I191" t="str">
-        <v>Wednesday</v>
+        <v>Friday</v>
       </c>
       <c r="J191" t="str">
-        <v>09:10</v>
+        <v>14:10</v>
       </c>
       <c r="K191" t="str">
-        <v>10:50</v>
+        <v>16:20</v>
       </c>
       <c r="L191">
         <v>2</v>
@@ -11090,10 +11090,10 @@
         <v>100</v>
       </c>
       <c r="N191">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O191">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="P191">
         <v>45</v>
@@ -11122,7 +11122,7 @@
         <v>MHA</v>
       </c>
       <c r="F192" t="str">
-        <v>CM-203</v>
+        <v>CM-102</v>
       </c>
       <c r="G192" t="str">
         <v>Non-Lab</v>
@@ -11134,10 +11134,10 @@
         <v>Wednesday</v>
       </c>
       <c r="J192" t="str">
-        <v>10:50</v>
+        <v>10:00</v>
       </c>
       <c r="K192" t="str">
-        <v>13:20</v>
+        <v>11:40</v>
       </c>
       <c r="L192">
         <v>2</v>
@@ -11146,10 +11146,10 @@
         <v>100</v>
       </c>
       <c r="N192">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O192">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="P192">
         <v>45</v>
@@ -11178,7 +11178,7 @@
         <v>TKN</v>
       </c>
       <c r="F193" t="str">
-        <v>G4-R1</v>
+        <v>G4-R4</v>
       </c>
       <c r="G193" t="str">
         <v>Non-Lab</v>
@@ -11190,10 +11190,10 @@
         <v>Wednesday</v>
       </c>
       <c r="J193" t="str">
-        <v>13:20</v>
+        <v>12:30</v>
       </c>
       <c r="K193" t="str">
-        <v>16:20</v>
+        <v>15:00</v>
       </c>
       <c r="L193">
         <v>3</v>
@@ -11202,10 +11202,10 @@
         <v>150</v>
       </c>
       <c r="N193">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O193">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P193">
         <v>56</v>
@@ -11234,7 +11234,7 @@
         <v>BMR</v>
       </c>
       <c r="F194" t="str">
-        <v>CM-207</v>
+        <v>G5-Lab1</v>
       </c>
       <c r="G194" t="str">
         <v>Lab</v>
@@ -11246,10 +11246,10 @@
         <v>Wednesday</v>
       </c>
       <c r="J194" t="str">
-        <v>16:20</v>
+        <v>15:30</v>
       </c>
       <c r="K194" t="str">
-        <v>19:20</v>
+        <v>18:00</v>
       </c>
       <c r="L194">
         <v>3</v>
@@ -11258,10 +11258,10 @@
         <v>150</v>
       </c>
       <c r="N194">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O194">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P194">
         <v>30</v>
@@ -11290,7 +11290,7 @@
         <v>BMR</v>
       </c>
       <c r="F195" t="str">
-        <v>G5-Lab1</v>
+        <v>CM-206</v>
       </c>
       <c r="G195" t="str">
         <v>Lab</v>
@@ -11302,10 +11302,10 @@
         <v>Tuesday</v>
       </c>
       <c r="J195" t="str">
-        <v>09:10</v>
+        <v>16:20</v>
       </c>
       <c r="K195" t="str">
-        <v>11:40</v>
+        <v>19:20</v>
       </c>
       <c r="L195">
         <v>3</v>
@@ -11314,10 +11314,10 @@
         <v>150</v>
       </c>
       <c r="N195">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O195">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="P195">
         <v>30</v>
@@ -11346,7 +11346,7 @@
         <v>MNI</v>
       </c>
       <c r="F196" t="str">
-        <v>CM-Lab3</v>
+        <v>G5-Lab2</v>
       </c>
       <c r="G196" t="str">
         <v>Lab</v>
@@ -11355,13 +11355,13 @@
         <v>No</v>
       </c>
       <c r="I196" t="str">
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="J196" t="str">
-        <v>07:30</v>
+        <v>09:10</v>
       </c>
       <c r="K196" t="str">
-        <v>10:00</v>
+        <v>11:40</v>
       </c>
       <c r="L196">
         <v>3</v>
@@ -11414,10 +11414,10 @@
         <v>Thursday</v>
       </c>
       <c r="J197" t="str">
-        <v>10:00</v>
+        <v>12:30</v>
       </c>
       <c r="K197" t="str">
-        <v>13:20</v>
+        <v>15:00</v>
       </c>
       <c r="L197">
         <v>3</v>
@@ -11426,10 +11426,10 @@
         <v>150</v>
       </c>
       <c r="N197">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O197">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="P197">
         <v>30</v>
@@ -11458,7 +11458,7 @@
         <v>BMR, ADF</v>
       </c>
       <c r="F198" t="str">
-        <v>G5-Lab2</v>
+        <v>CM-207</v>
       </c>
       <c r="G198" t="str">
         <v>Lab</v>
@@ -11470,10 +11470,10 @@
         <v>Thursday</v>
       </c>
       <c r="J198" t="str">
-        <v>14:10</v>
+        <v>15:30</v>
       </c>
       <c r="K198" t="str">
-        <v>17:10</v>
+        <v>18:00</v>
       </c>
       <c r="L198">
         <v>3</v>
@@ -11482,10 +11482,10 @@
         <v>150</v>
       </c>
       <c r="N198">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O198">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P198">
         <v>30</v>
@@ -11514,7 +11514,7 @@
         <v>BMR, ADF</v>
       </c>
       <c r="F199" t="str">
-        <v>G5-Lab2</v>
+        <v>CM-207</v>
       </c>
       <c r="G199" t="str">
         <v>Lab</v>
@@ -11523,13 +11523,13 @@
         <v>No</v>
       </c>
       <c r="I199" t="str">
-        <v>Tuesday</v>
+        <v>Friday</v>
       </c>
       <c r="J199" t="str">
-        <v>16:20</v>
+        <v>08:20</v>
       </c>
       <c r="K199" t="str">
-        <v>19:20</v>
+        <v>10:50</v>
       </c>
       <c r="L199">
         <v>3</v>
@@ -11538,10 +11538,10 @@
         <v>150</v>
       </c>
       <c r="N199">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O199">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="P199">
         <v>30</v>
@@ -11626,7 +11626,7 @@
         <v>ADF</v>
       </c>
       <c r="F201" t="str">
-        <v>G4-R3</v>
+        <v>G4-R4</v>
       </c>
       <c r="G201" t="str">
         <v>Non-Lab</v>
@@ -11682,7 +11682,7 @@
         <v>RNU</v>
       </c>
       <c r="F202" t="str">
-        <v>G4-R2</v>
+        <v>CM-204</v>
       </c>
       <c r="G202" t="str">
         <v>Non-Lab</v>
@@ -11694,10 +11694,10 @@
         <v>Monday</v>
       </c>
       <c r="J202" t="str">
-        <v>10:00</v>
+        <v>07:30</v>
       </c>
       <c r="K202" t="str">
-        <v>11:40</v>
+        <v>09:10</v>
       </c>
       <c r="L202">
         <v>2</v>
@@ -11738,7 +11738,7 @@
         <v>TAN</v>
       </c>
       <c r="F203" t="str">
-        <v>B3-R1</v>
+        <v>G4-R3</v>
       </c>
       <c r="G203" t="str">
         <v>Non-Lab</v>
@@ -11750,10 +11750,10 @@
         <v>Monday</v>
       </c>
       <c r="J203" t="str">
-        <v>07:30</v>
+        <v>09:10</v>
       </c>
       <c r="K203" t="str">
-        <v>10:00</v>
+        <v>11:40</v>
       </c>
       <c r="L203">
         <v>3</v>
@@ -11794,7 +11794,7 @@
         <v>RNA</v>
       </c>
       <c r="F204" t="str">
-        <v>CM-204</v>
+        <v>B3-R2</v>
       </c>
       <c r="G204" t="str">
         <v>Non-Lab</v>
@@ -11850,7 +11850,7 @@
         <v>MNR</v>
       </c>
       <c r="F205" t="str">
-        <v>G4-R1</v>
+        <v>CM-101</v>
       </c>
       <c r="G205" t="str">
         <v>Non-Lab</v>
@@ -11906,7 +11906,7 @@
         <v>MNR</v>
       </c>
       <c r="F206" t="str">
-        <v>G4-R4</v>
+        <v>B3-R2</v>
       </c>
       <c r="G206" t="str">
         <v>Non-Lab</v>
@@ -11915,13 +11915,13 @@
         <v>No</v>
       </c>
       <c r="I206" t="str">
-        <v>Tuesday</v>
+        <v>Wednesday</v>
       </c>
       <c r="J206" t="str">
-        <v>07:30</v>
+        <v>15:30</v>
       </c>
       <c r="K206" t="str">
-        <v>10:00</v>
+        <v>18:00</v>
       </c>
       <c r="L206">
         <v>3</v>
@@ -11962,7 +11962,7 @@
         <v>RNU</v>
       </c>
       <c r="F207" t="str">
-        <v>G2-R6</v>
+        <v>G4-R3</v>
       </c>
       <c r="G207" t="str">
         <v>Non-Lab</v>
@@ -12018,7 +12018,7 @@
         <v>ARI</v>
       </c>
       <c r="F208" t="str">
-        <v>G4-R1</v>
+        <v>G4-R3</v>
       </c>
       <c r="G208" t="str">
         <v>Non-Lab</v>
@@ -12074,7 +12074,7 @@
         <v>DAP</v>
       </c>
       <c r="F209" t="str">
-        <v>G2-R4</v>
+        <v>G3-R1</v>
       </c>
       <c r="G209" t="str">
         <v>Non-Lab</v>
@@ -12130,7 +12130,7 @@
         <v>RNA</v>
       </c>
       <c r="F210" t="str">
-        <v>B2-R1</v>
+        <v>B3-R2</v>
       </c>
       <c r="G210" t="str">
         <v>Non-Lab</v>
@@ -12186,7 +12186,7 @@
         <v>DAP</v>
       </c>
       <c r="F211" t="str">
-        <v>G2-R4</v>
+        <v>CM-203</v>
       </c>
       <c r="G211" t="str">
         <v>Non-Lab</v>
@@ -12242,7 +12242,7 @@
         <v>MNR</v>
       </c>
       <c r="F212" t="str">
-        <v>G5-Lab1</v>
+        <v>G5-LabAudioVisual</v>
       </c>
       <c r="G212" t="str">
         <v>Lab</v>
@@ -12251,13 +12251,13 @@
         <v>No</v>
       </c>
       <c r="I212" t="str">
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="J212" t="str">
-        <v>15:30</v>
+        <v>07:30</v>
       </c>
       <c r="K212" t="str">
-        <v>18:00</v>
+        <v>10:00</v>
       </c>
       <c r="L212">
         <v>3</v>
@@ -12298,7 +12298,7 @@
         <v>TAN</v>
       </c>
       <c r="F213" t="str">
-        <v>G3-R2</v>
+        <v>B3-R2</v>
       </c>
       <c r="G213" t="str">
         <v>Non-Lab</v>
@@ -12354,7 +12354,7 @@
         <v>RNA</v>
       </c>
       <c r="F214" t="str">
-        <v>G3-R1</v>
+        <v>CM-205</v>
       </c>
       <c r="G214" t="str">
         <v>Non-Lab</v>
@@ -12366,10 +12366,10 @@
         <v>Thursday</v>
       </c>
       <c r="J214" t="str">
-        <v>10:00</v>
+        <v>13:20</v>
       </c>
       <c r="K214" t="str">
-        <v>13:20</v>
+        <v>16:20</v>
       </c>
       <c r="L214">
         <v>3</v>
@@ -12378,10 +12378,10 @@
         <v>150</v>
       </c>
       <c r="N214">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="O214">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="P214">
         <v>30</v>
@@ -12410,7 +12410,7 @@
         <v>MHA</v>
       </c>
       <c r="F215" t="str">
-        <v>CM-208</v>
+        <v>CM-101</v>
       </c>
       <c r="G215" t="str">
         <v>Non-Lab</v>
@@ -12466,7 +12466,7 @@
         <v>TAN</v>
       </c>
       <c r="F216" t="str">
-        <v>CM-101</v>
+        <v>CM-203</v>
       </c>
       <c r="G216" t="str">
         <v>Non-Lab</v>
@@ -12522,7 +12522,7 @@
         <v>RNU</v>
       </c>
       <c r="F217" t="str">
-        <v>CM-202</v>
+        <v>CM-201</v>
       </c>
       <c r="G217" t="str">
         <v>Non-Lab</v>
@@ -12534,11 +12534,11 @@
         <v>Thursday</v>
       </c>
       <c r="J217" t="str">
+        <v>10:00</v>
+      </c>
+      <c r="K217" t="str">
         <v>13:20</v>
       </c>
-      <c r="K217" t="str">
-        <v>16:20</v>
-      </c>
       <c r="L217">
         <v>3</v>
       </c>
@@ -12546,10 +12546,10 @@
         <v>150</v>
       </c>
       <c r="N217">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O217">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="P217">
         <v>40</v>
@@ -12578,7 +12578,7 @@
         <v>TAN</v>
       </c>
       <c r="F218" t="str">
-        <v>CM-202</v>
+        <v>CM-203</v>
       </c>
       <c r="G218" t="str">
         <v>Non-Lab</v>
@@ -12634,7 +12634,7 @@
         <v>RNA</v>
       </c>
       <c r="F219" t="str">
-        <v>CM-203</v>
+        <v>CM-102</v>
       </c>
       <c r="G219" t="str">
         <v>Non-Lab</v>

</xml_diff>